<commit_message>
Fixed grid mean and velocity byEndmember
SelPoints wasn't being appended but was being overwritten
</commit_message>
<xml_diff>
--- a/Data/Drifter deployment checklist.xlsx
+++ b/Data/Drifter deployment checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\samoa\DRIFTERS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Faga-alu-Bay-water-circulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="136">
   <si>
     <t>Swell</t>
   </si>
@@ -404,9 +404,6 @@
     <t>#27,#28</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>wind</t>
   </si>
   <si>
@@ -422,13 +419,22 @@
     <t>4,5,7,8</t>
   </si>
   <si>
-    <t>wa</t>
+    <t>*only drifters D1,D3,D4,D5-D1 has some weird issue in the middle of it</t>
   </si>
   <si>
-    <t>wi</t>
+    <t>Julian(local)</t>
   </si>
   <si>
-    <t>*only drifters D1,D3,D4,D5-D1 has some weird issue in the middle of it</t>
+    <t>EndMember</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>tide</t>
   </si>
 </sst>
 </file>
@@ -710,36 +716,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -769,19 +745,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -887,12 +850,36 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
-      </right>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -905,9 +892,18 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -921,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1032,20 +1028,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1089,7 +1079,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1101,67 +1091,52 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1184,6 +1159,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2020,1784 +2019,1948 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="8" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="31" t="s">
-        <v>111</v>
-      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
       <c r="P1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="90" t="s">
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="D2" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="J2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="O2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="73" t="s">
+      <c r="Q2" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="R2" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="50">
+        <v>135</v>
+      </c>
+      <c r="C3" s="98">
         <v>1</v>
       </c>
-      <c r="C3" s="87">
+      <c r="D3" s="104">
+        <v>19</v>
+      </c>
+      <c r="E3" s="84">
         <v>41658</v>
       </c>
-      <c r="D3" s="75">
+      <c r="F3" s="73">
         <v>1300</v>
       </c>
-      <c r="E3" s="75">
+      <c r="G3" s="73">
         <v>1500</v>
       </c>
-      <c r="F3" s="13">
+      <c r="H3" s="13">
         <f>'NDBC NSTP6 timeseries data'!I4</f>
         <v>1.5389999999999999</v>
       </c>
-      <c r="G3" s="13">
+      <c r="I3" s="13">
         <f>'NDBC NSTP6 timeseries data'!I24</f>
         <v>0.97399999999999998</v>
       </c>
-      <c r="H3" s="47">
-        <f>G3-F3</f>
+      <c r="J3" s="47">
+        <f>I3-H3</f>
         <v>-0.56499999999999995</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="48">
+      <c r="L3" s="48">
         <f>'NDBC NSTP6 timeseries data'!K25</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K3" s="49">
+      <c r="M3" s="49">
         <f>'NDBC NSTP6 timeseries data'!L25</f>
         <v>232.5</v>
       </c>
-      <c r="L3" s="48">
+      <c r="N3" s="48">
         <f>'NDBC NSTP6 timeseries data'!M25</f>
         <v>3.6</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="O3" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="77" t="s">
+      <c r="P3" s="13"/>
+      <c r="Q3" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="R3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="51">
-        <f>B3+1</f>
+        <v>135</v>
+      </c>
+      <c r="C4" s="99">
+        <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="88">
+      <c r="D4" s="104">
+        <v>20</v>
+      </c>
+      <c r="E4" s="85">
         <v>41659</v>
       </c>
-      <c r="D4" s="74">
+      <c r="F4" s="72">
         <v>1615</v>
       </c>
-      <c r="E4" s="74">
+      <c r="G4" s="72">
         <v>1730</v>
       </c>
-      <c r="F4" s="11">
+      <c r="H4" s="11">
         <f>'NDBC NSTP6 timeseries data'!I27</f>
         <v>1.03</v>
       </c>
-      <c r="G4" s="11">
+      <c r="I4" s="11">
         <f>'NDBC NSTP6 timeseries data'!I42</f>
         <v>1.23</v>
       </c>
-      <c r="H4" s="32">
-        <f>G4-F4</f>
+      <c r="J4" s="32">
+        <f>I4-H4</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="28">
+      <c r="L4" s="28">
         <f>'NDBC NSTP6 timeseries data'!K43</f>
         <v>2.375</v>
       </c>
-      <c r="K4" s="27">
+      <c r="M4" s="27">
         <f>'NDBC NSTP6 timeseries data'!L43</f>
         <v>193.6875</v>
       </c>
-      <c r="L4" s="28">
+      <c r="N4" s="28">
         <f>'NDBC NSTP6 timeseries data'!M43</f>
         <v>7</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="77" t="s">
+      <c r="P4" s="11"/>
+      <c r="Q4" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="R4" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="51">
-        <f>B4+1</f>
+        <v>135</v>
+      </c>
+      <c r="C5" s="99">
+        <f>C4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="88">
+      <c r="D5" s="104">
+        <v>20</v>
+      </c>
+      <c r="E5" s="85">
         <v>41659</v>
       </c>
-      <c r="D5" s="74">
+      <c r="F5" s="72">
         <v>1750</v>
       </c>
-      <c r="E5" s="74">
+      <c r="G5" s="72">
         <v>1900</v>
       </c>
-      <c r="F5" s="11">
+      <c r="H5" s="11">
         <f>'NDBC NSTP6 timeseries data'!I45</f>
         <v>1.23</v>
       </c>
-      <c r="G5" s="11">
+      <c r="I5" s="11">
         <f>'NDBC NSTP6 timeseries data'!I60</f>
         <v>1.94</v>
       </c>
-      <c r="H5" s="32">
-        <f t="shared" ref="H5" si="0">G5-F5</f>
+      <c r="J5" s="32">
+        <f t="shared" ref="J5" si="0">I5-H5</f>
         <v>0.71</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="28">
+      <c r="L5" s="28">
         <f>'NDBC NSTP6 timeseries data'!K61</f>
         <v>3.25</v>
       </c>
-      <c r="K5" s="27">
+      <c r="M5" s="27">
         <f>'NDBC NSTP6 timeseries data'!L61</f>
         <v>258.375</v>
       </c>
-      <c r="L5" s="28">
+      <c r="N5" s="28">
         <f>'NDBC NSTP6 timeseries data'!M61</f>
         <v>10</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="O5" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="77" t="s">
+      <c r="P5" s="11"/>
+      <c r="Q5" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="R5" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="51">
-        <f t="shared" ref="B6:B32" si="1">B5+1</f>
+        <v>125</v>
+      </c>
+      <c r="C6" s="99">
+        <f t="shared" ref="C6:C32" si="1">C5+1</f>
         <v>4</v>
       </c>
-      <c r="C6" s="88">
+      <c r="D6" s="104">
+        <v>32</v>
+      </c>
+      <c r="E6" s="85">
         <v>41671</v>
       </c>
-      <c r="D6" s="74">
+      <c r="F6" s="72">
         <v>900</v>
       </c>
-      <c r="E6" s="74">
+      <c r="G6" s="72">
         <v>1100</v>
       </c>
-      <c r="F6" s="11">
+      <c r="H6" s="11">
         <v>3.7429999999999999</v>
       </c>
-      <c r="G6" s="11">
+      <c r="I6" s="11">
         <v>2.58</v>
       </c>
-      <c r="H6" s="72">
-        <f>G6-F6</f>
+      <c r="J6" s="70">
+        <f>I6-H6</f>
         <v>-1.1629999999999998</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="28">
+      <c r="L6" s="28">
         <f>'NDBC NSTP6 timeseries data'!K84</f>
         <v>5.2725</v>
       </c>
-      <c r="K6" s="27">
+      <c r="M6" s="27">
         <f>'NDBC NSTP6 timeseries data'!L84</f>
         <v>96.1875</v>
       </c>
-      <c r="L6" s="28">
+      <c r="N6" s="28">
         <f>'NDBC NSTP6 timeseries data'!M84</f>
         <v>11.08</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="O6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="77" t="s">
+      <c r="P6" s="11"/>
+      <c r="Q6" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="R6" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="51">
+        <v>125</v>
+      </c>
+      <c r="C7" s="99">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C7" s="88">
+      <c r="D7" s="104">
+        <v>32</v>
+      </c>
+      <c r="E7" s="85">
         <v>41671</v>
       </c>
-      <c r="D7" s="74">
+      <c r="F7" s="72">
         <v>1130</v>
       </c>
-      <c r="E7" s="74">
+      <c r="G7" s="72">
         <v>1300</v>
       </c>
-      <c r="F7" s="11">
+      <c r="H7" s="11">
         <v>2.2280000000000002</v>
       </c>
-      <c r="G7" s="11">
+      <c r="I7" s="11">
         <v>0.879</v>
       </c>
-      <c r="H7" s="72">
-        <f>G7-F7</f>
+      <c r="J7" s="70">
+        <f>I7-H7</f>
         <v>-1.3490000000000002</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="28">
+      <c r="L7" s="28">
         <f>'NDBC NSTP6 timeseries data'!K102</f>
         <v>5.6875</v>
       </c>
-      <c r="K7" s="27">
+      <c r="M7" s="27">
         <f>'NDBC NSTP6 timeseries data'!L102</f>
         <v>100.25</v>
       </c>
-      <c r="L7" s="28">
+      <c r="N7" s="28">
         <f>'NDBC NSTP6 timeseries data'!M102</f>
         <v>13</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="77" t="s">
+      <c r="P7" s="11"/>
+      <c r="Q7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="R7" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="51">
+        <v>125</v>
+      </c>
+      <c r="C8" s="99">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C8" s="88">
+      <c r="D8" s="104">
+        <v>32</v>
+      </c>
+      <c r="E8" s="85">
         <v>41671</v>
       </c>
-      <c r="D8" s="74">
+      <c r="F8" s="72">
         <v>1700</v>
       </c>
-      <c r="E8" s="74">
+      <c r="G8" s="72">
         <v>1900</v>
       </c>
-      <c r="F8" s="11">
+      <c r="H8" s="11">
         <v>1.512</v>
       </c>
-      <c r="G8" s="11">
+      <c r="I8" s="11">
         <v>3.222</v>
       </c>
-      <c r="H8" s="32">
-        <f t="shared" ref="H8:H32" si="2">G8-F8</f>
+      <c r="J8" s="32">
+        <f t="shared" ref="J8:J32" si="2">I8-H8</f>
         <v>1.71</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="28">
+      <c r="L8" s="28">
         <f>'NDBC NSTP6 timeseries data'!K125</f>
         <v>4.2380952380952381</v>
       </c>
-      <c r="K8" s="27">
+      <c r="M8" s="27">
         <f>'NDBC NSTP6 timeseries data'!L125</f>
         <v>187.95238095238096</v>
       </c>
-      <c r="L8" s="28">
+      <c r="N8" s="28">
         <f>'NDBC NSTP6 timeseries data'!M125</f>
         <v>13</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="77" t="s">
+      <c r="P8" s="11"/>
+      <c r="Q8" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="R8" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="51">
+        <v>125</v>
+      </c>
+      <c r="C9" s="99">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C9" s="88">
+      <c r="D9" s="104">
+        <v>39</v>
+      </c>
+      <c r="E9" s="85">
         <v>41678</v>
       </c>
-      <c r="D9" s="74">
+      <c r="F9" s="72">
         <v>1415</v>
       </c>
-      <c r="E9" s="74">
+      <c r="G9" s="72">
         <v>1545</v>
       </c>
-      <c r="F9" s="11">
+      <c r="H9" s="11">
         <f>'NDBC NSTP6 timeseries data'!I127</f>
         <v>3.1</v>
       </c>
-      <c r="G9" s="11">
+      <c r="I9" s="11">
         <f>'NDBC NSTP6 timeseries data'!I143</f>
         <v>3.45</v>
       </c>
-      <c r="H9" s="32">
+      <c r="J9" s="32">
         <f t="shared" si="2"/>
         <v>0.35000000000000009</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="28">
+      <c r="L9" s="28">
         <f>'NDBC NSTP6 timeseries data'!K144</f>
         <v>5.2352941176470589</v>
       </c>
-      <c r="K9" s="27">
+      <c r="M9" s="27">
         <f>'NDBC NSTP6 timeseries data'!L144</f>
         <v>140.41176470588235</v>
       </c>
-      <c r="L9" s="28">
+      <c r="N9" s="28">
         <f>'NDBC NSTP6 timeseries data'!M144</f>
         <v>18</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="O9" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="77" t="s">
+      <c r="P9" s="11"/>
+      <c r="Q9" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="R9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q9" s="91" t="s">
+      <c r="S9" s="88" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="51">
+        <v>125</v>
+      </c>
+      <c r="C10" s="99">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C10" s="88">
+      <c r="D10" s="104">
+        <v>39</v>
+      </c>
+      <c r="E10" s="85">
         <v>41678</v>
       </c>
-      <c r="D10" s="74">
+      <c r="F10" s="72">
         <v>1605</v>
       </c>
-      <c r="E10" s="74">
+      <c r="G10" s="72">
         <v>1800</v>
       </c>
-      <c r="F10" s="11">
+      <c r="H10" s="11">
         <f>'NDBC NSTP6 timeseries data'!I146</f>
         <v>3.33</v>
       </c>
-      <c r="G10" s="11">
+      <c r="I10" s="11">
         <f>'NDBC NSTP6 timeseries data'!I167</f>
         <v>2.5299999999999998</v>
       </c>
-      <c r="H10" s="72">
+      <c r="J10" s="70">
         <f t="shared" si="2"/>
         <v>-0.80000000000000027</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="28">
+      <c r="L10" s="28">
         <f>'NDBC NSTP6 timeseries data'!K168</f>
         <v>6.0454545454545459</v>
       </c>
-      <c r="K10" s="27">
+      <c r="M10" s="27">
         <f>'NDBC NSTP6 timeseries data'!L168</f>
         <v>144.13636363636363</v>
       </c>
-      <c r="L10" s="28">
+      <c r="N10" s="28">
         <f>'NDBC NSTP6 timeseries data'!M168</f>
         <v>20</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="O10" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N10" s="11"/>
-      <c r="O10" s="77" t="s">
+      <c r="P10" s="11"/>
+      <c r="Q10" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="R10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q10" s="91" t="s">
+      <c r="S10" s="88" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="51">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="99">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C11" s="88">
+      <c r="D11" s="104">
+        <v>47</v>
+      </c>
+      <c r="E11" s="85">
         <v>41686</v>
       </c>
-      <c r="D11" s="74">
+      <c r="F11" s="72">
         <v>1654</v>
       </c>
-      <c r="E11" s="74">
+      <c r="G11" s="72">
         <v>1846</v>
       </c>
-      <c r="F11" s="11">
+      <c r="H11" s="11">
         <f>'NDBC NSTP6 timeseries data'!I170</f>
         <v>2.39</v>
       </c>
-      <c r="G11" s="11">
+      <c r="I11" s="11">
         <f>'NDBC NSTP6 timeseries data'!I189</f>
         <v>3.25</v>
       </c>
-      <c r="H11" s="32">
+      <c r="J11" s="32">
         <f t="shared" si="2"/>
         <v>0.85999999999999988</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="28">
+      <c r="L11" s="28">
         <f>'NDBC NSTP6 timeseries data'!K190</f>
         <v>3.25</v>
       </c>
-      <c r="K11" s="27">
+      <c r="M11" s="27">
         <f>'NDBC NSTP6 timeseries data'!L190</f>
         <v>168.8</v>
       </c>
-      <c r="L11" s="28">
+      <c r="N11" s="28">
         <f>'NDBC NSTP6 timeseries data'!M190</f>
         <v>9</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N11" s="11"/>
-      <c r="O11" s="77" t="s">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="R11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="91" t="s">
+      <c r="S11" s="88" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="51">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="99">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C12" s="88">
+      <c r="D12" s="104">
+        <v>48</v>
+      </c>
+      <c r="E12" s="85">
         <v>41687</v>
       </c>
-      <c r="D12" s="74">
+      <c r="F12" s="72">
         <v>1245</v>
       </c>
-      <c r="E12" s="74">
+      <c r="G12" s="72">
         <v>1500</v>
       </c>
-      <c r="F12" s="11">
+      <c r="H12" s="11">
         <f>'NDBC NSTP6 timeseries data'!I192</f>
         <v>1.62</v>
       </c>
-      <c r="G12" s="11">
+      <c r="I12" s="11">
         <f>'NDBC NSTP6 timeseries data'!I215</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="H12" s="72">
+      <c r="J12" s="70">
         <f t="shared" si="2"/>
         <v>-0.51</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="28">
+      <c r="L12" s="28">
         <f>'NDBC NSTP6 timeseries data'!K216</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="K12" s="27">
+      <c r="M12" s="27">
         <f>'NDBC NSTP6 timeseries data'!L216</f>
         <v>79.958333333333329</v>
       </c>
-      <c r="L12" s="28">
+      <c r="N12" s="28">
         <f>'NDBC NSTP6 timeseries data'!M216</f>
         <v>28</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="77" t="s">
+      <c r="P12" s="11"/>
+      <c r="Q12" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="R12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q12" s="91" t="s">
+      <c r="S12" s="88" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="51">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="99">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C13" s="88">
+      <c r="D13" s="104">
+        <v>48</v>
+      </c>
+      <c r="E13" s="85">
         <v>41687</v>
       </c>
-      <c r="D13" s="74">
+      <c r="F13" s="72">
         <v>1530</v>
       </c>
-      <c r="E13" s="74">
+      <c r="G13" s="72">
         <v>1700</v>
       </c>
-      <c r="F13" s="11">
+      <c r="H13" s="11">
         <f>'NDBC NSTP6 timeseries data'!I218</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="G13" s="11">
+      <c r="I13" s="11">
         <f>'NDBC NSTP6 timeseries data'!I236</f>
         <v>1.59</v>
       </c>
-      <c r="H13" s="32">
+      <c r="J13" s="32">
         <f t="shared" si="2"/>
         <v>0.45000000000000018</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="28">
+      <c r="L13" s="28">
         <f>'NDBC NSTP6 timeseries data'!K237</f>
         <v>5.8947368421052628</v>
       </c>
-      <c r="K13" s="27">
+      <c r="M13" s="27">
         <f>'NDBC NSTP6 timeseries data'!L237</f>
         <v>101.36842105263158</v>
       </c>
-      <c r="L13" s="28">
+      <c r="N13" s="28">
         <f>'NDBC NSTP6 timeseries data'!M237</f>
         <v>20</v>
       </c>
-      <c r="M13" s="12" t="s">
+      <c r="O13" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N13" s="11"/>
-      <c r="O13" s="77" t="s">
+      <c r="P13" s="11"/>
+      <c r="Q13" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="R13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q13" s="91" t="s">
+      <c r="S13" s="88" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="51">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="99">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C14" s="88">
+      <c r="D14" s="104">
+        <v>48</v>
+      </c>
+      <c r="E14" s="85">
         <v>41687</v>
       </c>
-      <c r="D14" s="74">
+      <c r="F14" s="72">
         <v>1710</v>
       </c>
-      <c r="E14" s="74">
+      <c r="G14" s="72">
         <v>1840</v>
       </c>
-      <c r="F14" s="11">
+      <c r="H14" s="11">
         <f>'NDBC NSTP6 timeseries data'!I239</f>
         <v>1.62</v>
       </c>
-      <c r="G14" s="11">
+      <c r="I14" s="11">
         <f>'NDBC NSTP6 timeseries data'!I256</f>
         <v>2.56</v>
       </c>
-      <c r="H14" s="32">
+      <c r="J14" s="32">
         <f t="shared" si="2"/>
         <v>0.94</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="28">
+      <c r="L14" s="28">
         <f>'NDBC NSTP6 timeseries data'!K257</f>
         <v>5.166666666666667</v>
       </c>
-      <c r="K14" s="27">
+      <c r="M14" s="27">
         <f>'NDBC NSTP6 timeseries data'!L257</f>
         <v>89.888888888888886</v>
       </c>
-      <c r="L14" s="28">
+      <c r="N14" s="28">
         <f>'NDBC NSTP6 timeseries data'!M257</f>
         <v>15</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="O14" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="77" t="s">
+      <c r="P14" s="11"/>
+      <c r="Q14" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="R14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q14" s="91" t="s">
+      <c r="S14" s="88" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="51">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="99">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C15" s="88">
+      <c r="D15" s="104">
+        <v>49</v>
+      </c>
+      <c r="E15" s="85">
         <v>41688</v>
       </c>
-      <c r="D15" s="74">
+      <c r="F15" s="72">
         <v>1245</v>
       </c>
-      <c r="E15" s="74">
+      <c r="G15" s="72">
         <v>1445</v>
       </c>
-      <c r="F15" s="11">
+      <c r="H15" s="11">
         <f>'NDBC NSTP6 timeseries data'!I259</f>
         <v>2.09</v>
       </c>
-      <c r="G15" s="11">
+      <c r="I15" s="11">
         <f>'NDBC NSTP6 timeseries data'!I280</f>
         <v>1.26</v>
       </c>
-      <c r="H15" s="72">
+      <c r="J15" s="70">
         <f t="shared" si="2"/>
         <v>-0.82999999999999985</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="K15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="28">
+      <c r="L15" s="28">
         <f>'NDBC NSTP6 timeseries data'!K281</f>
         <v>4.9090909090909092</v>
       </c>
-      <c r="K15" s="27">
+      <c r="M15" s="27">
         <f>'NDBC NSTP6 timeseries data'!L281</f>
         <v>97.727272727272734</v>
       </c>
-      <c r="L15" s="28">
+      <c r="N15" s="28">
         <f>'NDBC NSTP6 timeseries data'!M281</f>
         <v>14</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="O15" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N15" s="11"/>
-      <c r="O15" s="77" t="s">
+      <c r="P15" s="11"/>
+      <c r="Q15" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="15" t="s">
+      <c r="R15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q15" s="91" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S15" s="88" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B16" s="78">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="100">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C16" s="89">
+      <c r="D16" s="104">
+        <v>49</v>
+      </c>
+      <c r="E16" s="86">
         <v>41688</v>
       </c>
-      <c r="D16" s="79">
+      <c r="F16" s="76">
         <v>1445</v>
       </c>
-      <c r="E16" s="79">
+      <c r="G16" s="76">
         <v>1700</v>
       </c>
-      <c r="F16" s="80">
+      <c r="H16" s="77">
         <f>'NDBC NSTP6 timeseries data'!I283</f>
         <v>1.3</v>
       </c>
-      <c r="G16" s="80">
+      <c r="I16" s="77">
         <f>'NDBC NSTP6 timeseries data'!I306</f>
         <v>1.37</v>
       </c>
-      <c r="H16" s="81">
+      <c r="J16" s="78">
         <f t="shared" si="2"/>
         <v>7.0000000000000062E-2</v>
       </c>
-      <c r="I16" s="80" t="s">
+      <c r="K16" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="J16" s="82">
+      <c r="L16" s="79">
         <f>'NDBC NSTP6 timeseries data'!K307</f>
         <v>4.708333333333333</v>
       </c>
-      <c r="K16" s="83">
+      <c r="M16" s="80">
         <f>'NDBC NSTP6 timeseries data'!L307</f>
         <v>194.41666666666666</v>
       </c>
-      <c r="L16" s="82">
+      <c r="N16" s="79">
         <f>'NDBC NSTP6 timeseries data'!M307</f>
         <v>15</v>
       </c>
-      <c r="M16" s="84" t="s">
+      <c r="O16" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="80"/>
-      <c r="O16" s="85" t="s">
+      <c r="P16" s="77"/>
+      <c r="Q16" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P16" s="92" t="s">
+      <c r="R16" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="91" t="s">
+      <c r="S16" s="88" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="51">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="99">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C17" s="88">
+      <c r="D17" s="104">
+        <v>50</v>
+      </c>
+      <c r="E17" s="85">
         <v>41689</v>
       </c>
-      <c r="D17" s="74">
+      <c r="F17" s="72">
         <v>1205</v>
       </c>
-      <c r="E17" s="74">
+      <c r="G17" s="72">
         <v>1440</v>
       </c>
-      <c r="F17" s="11">
+      <c r="H17" s="11">
         <f>'NDBC NSTP6 timeseries data'!I309</f>
         <v>2.8809999999999998</v>
       </c>
-      <c r="G17" s="11">
+      <c r="I17" s="11">
         <f>'NDBC NSTP6 timeseries data'!I336</f>
         <v>1.516</v>
       </c>
-      <c r="H17" s="93">
+      <c r="J17" s="90">
         <f t="shared" si="2"/>
         <v>-1.3649999999999998</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="28">
+      <c r="L17" s="28">
         <f>'NDBC NSTP6 timeseries data'!K337</f>
         <v>5.7757142857142858</v>
       </c>
-      <c r="K17" s="27">
+      <c r="M17" s="27">
         <f>'NDBC NSTP6 timeseries data'!L337</f>
         <v>39.857142857142854</v>
       </c>
-      <c r="L17" s="28">
+      <c r="N17" s="28">
         <f>'NDBC NSTP6 timeseries data'!M337</f>
         <v>11.47</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="O17" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N17" s="11"/>
-      <c r="O17" s="85" t="s">
+      <c r="P17" s="11"/>
+      <c r="Q17" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P17" s="92" t="s">
+      <c r="R17" s="89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="51">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="99">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C18" s="88">
+      <c r="D18" s="104">
+        <v>50</v>
+      </c>
+      <c r="E18" s="85">
         <v>41689</v>
       </c>
-      <c r="D18" s="74">
+      <c r="F18" s="72">
         <v>1445</v>
       </c>
-      <c r="E18" s="74">
+      <c r="G18" s="72">
         <v>1720</v>
       </c>
-      <c r="F18" s="11">
+      <c r="H18" s="11">
         <f>'NDBC NSTP6 timeseries data'!I339</f>
         <v>1.516</v>
       </c>
-      <c r="G18" s="11">
+      <c r="I18" s="11">
         <f>'NDBC NSTP6 timeseries data'!I365</f>
         <v>1.24</v>
       </c>
-      <c r="H18" s="93">
+      <c r="J18" s="90">
         <f t="shared" si="2"/>
         <v>-0.27600000000000002</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="K18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="28">
+      <c r="L18" s="28">
         <f>'NDBC NSTP6 timeseries data'!K366</f>
         <v>6.565555555555556</v>
       </c>
-      <c r="K18" s="27">
+      <c r="M18" s="27">
         <f>'NDBC NSTP6 timeseries data'!L366</f>
         <v>54.407407407407405</v>
       </c>
-      <c r="L18" s="28">
+      <c r="N18" s="28">
         <f>'NDBC NSTP6 timeseries data'!M366</f>
         <v>14.77</v>
       </c>
-      <c r="M18" s="12" t="s">
+      <c r="O18" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="77" t="s">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="R18" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="51">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="99">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C19" s="88">
+      <c r="D19" s="104">
+        <v>51</v>
+      </c>
+      <c r="E19" s="85">
         <v>41690</v>
       </c>
-      <c r="D19" s="74">
+      <c r="F19" s="72">
         <v>840</v>
       </c>
-      <c r="E19" s="74">
+      <c r="G19" s="72">
         <v>1045</v>
       </c>
-      <c r="F19" s="11">
+      <c r="H19" s="11">
         <f>'NDBC NSTP6 timeseries data'!I368</f>
         <v>2.52</v>
       </c>
-      <c r="G19" s="11">
+      <c r="I19" s="11">
         <f>'NDBC NSTP6 timeseries data'!I389</f>
         <v>3.15</v>
       </c>
-      <c r="H19" s="81">
+      <c r="J19" s="78">
         <f t="shared" si="2"/>
         <v>0.62999999999999989</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="28">
+      <c r="L19" s="28">
         <f>'NDBC NSTP6 timeseries data'!K390</f>
         <v>4.8181818181818183</v>
       </c>
-      <c r="K19" s="27">
+      <c r="M19" s="27">
         <f>'NDBC NSTP6 timeseries data'!L390</f>
         <v>290.22727272727275</v>
       </c>
-      <c r="L19" s="28">
+      <c r="N19" s="28">
         <f>'NDBC NSTP6 timeseries data'!M390</f>
         <v>13</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="O19" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="85" t="s">
+      <c r="P19" s="11"/>
+      <c r="Q19" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P19" s="92" t="s">
+      <c r="R19" s="89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="51">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="99">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C20" s="88">
+      <c r="D20" s="104">
+        <v>51</v>
+      </c>
+      <c r="E20" s="85">
         <v>41690</v>
       </c>
-      <c r="D20" s="74">
+      <c r="F20" s="72">
         <v>1100</v>
       </c>
-      <c r="E20" s="74">
+      <c r="G20" s="72">
         <v>1200</v>
       </c>
-      <c r="F20" s="11">
+      <c r="H20" s="11">
         <f>'NDBC NSTP6 timeseries data'!I392</f>
         <v>3.2</v>
       </c>
-      <c r="G20" s="11">
+      <c r="I20" s="11">
         <f>'NDBC NSTP6 timeseries data'!I402</f>
         <v>3.05</v>
       </c>
-      <c r="H20" s="93">
+      <c r="J20" s="90">
         <f t="shared" si="2"/>
         <v>-0.15000000000000036</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="28">
+      <c r="L20" s="28">
         <f>'NDBC NSTP6 timeseries data'!K403</f>
         <v>4.2727272727272725</v>
       </c>
-      <c r="K20" s="27">
+      <c r="M20" s="27">
         <f>'NDBC NSTP6 timeseries data'!L403</f>
         <v>117.18181818181819</v>
       </c>
-      <c r="L20" s="28">
+      <c r="N20" s="28">
         <f>'NDBC NSTP6 timeseries data'!M403</f>
         <v>11</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="O20" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="85" t="s">
+      <c r="P20" s="11"/>
+      <c r="Q20" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="92" t="s">
+      <c r="R20" s="89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="51">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="99">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C21" s="88">
+      <c r="D21" s="104">
+        <v>51</v>
+      </c>
+      <c r="E21" s="85">
         <v>41690</v>
       </c>
-      <c r="D21" s="74">
+      <c r="F21" s="72">
         <v>1210</v>
       </c>
-      <c r="E21" s="74">
+      <c r="G21" s="72">
         <v>1430</v>
       </c>
-      <c r="F21" s="11">
+      <c r="H21" s="11">
         <f>'NDBC NSTP6 timeseries data'!I405</f>
         <v>3.02</v>
       </c>
-      <c r="G21" s="11">
+      <c r="I21" s="11">
         <f>'NDBC NSTP6 timeseries data'!I429</f>
         <v>2.06</v>
       </c>
-      <c r="H21" s="93">
+      <c r="J21" s="90">
         <f t="shared" si="2"/>
         <v>-0.96</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="28">
+      <c r="L21" s="28">
         <f>'NDBC NSTP6 timeseries data'!K430</f>
         <v>2.96</v>
       </c>
-      <c r="K21" s="27">
+      <c r="M21" s="27">
         <f>'NDBC NSTP6 timeseries data'!L430</f>
         <v>237.8</v>
       </c>
-      <c r="L21" s="28">
+      <c r="N21" s="28">
         <f>'NDBC NSTP6 timeseries data'!M430</f>
         <v>12</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="O21" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="77" t="s">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P21" s="15" t="s">
+      <c r="R21" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" s="51">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="99">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C22" s="88">
+      <c r="D22" s="104">
+        <v>51</v>
+      </c>
+      <c r="E22" s="85">
         <v>41690</v>
       </c>
-      <c r="D22" s="74">
+      <c r="F22" s="72">
         <v>1500</v>
       </c>
-      <c r="E22" s="74">
+      <c r="G22" s="72">
         <v>1630</v>
       </c>
-      <c r="F22" s="11">
+      <c r="H22" s="11">
         <f>'NDBC NSTP6 timeseries data'!I432</f>
         <v>1.85</v>
       </c>
-      <c r="G22" s="11">
+      <c r="I22" s="11">
         <f>'NDBC NSTP6 timeseries data'!I447</f>
         <v>1.29</v>
       </c>
-      <c r="H22" s="93">
+      <c r="J22" s="90">
         <f t="shared" si="2"/>
         <v>-0.56000000000000005</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="28">
+      <c r="L22" s="28">
         <f>'NDBC NSTP6 timeseries data'!K448</f>
         <v>5.9375</v>
       </c>
-      <c r="K22" s="27">
+      <c r="M22" s="27">
         <f>'NDBC NSTP6 timeseries data'!L448</f>
         <v>290</v>
       </c>
-      <c r="L22" s="28">
+      <c r="N22" s="28">
         <f>'NDBC NSTP6 timeseries data'!M448</f>
         <v>13</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="O22" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="77" t="s">
+      <c r="P22" s="11"/>
+      <c r="Q22" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="P22" s="15" t="s">
+      <c r="R22" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="51">
+        <v>135</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="99">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="C23" s="88">
+      <c r="D23" s="104">
+        <v>52</v>
+      </c>
+      <c r="E23" s="85">
         <v>41691</v>
       </c>
-      <c r="D23" s="11">
+      <c r="F23" s="11">
         <v>920</v>
       </c>
-      <c r="E23" s="11">
+      <c r="G23" s="11">
         <v>1040</v>
       </c>
-      <c r="F23" s="11">
+      <c r="H23" s="11">
         <f>'NDBC NSTP6 timeseries data'!I450</f>
         <v>2.37</v>
       </c>
-      <c r="G23" s="11">
+      <c r="I23" s="11">
         <f>'NDBC NSTP6 timeseries data'!I464</f>
         <v>2.97</v>
       </c>
-      <c r="H23" s="81">
+      <c r="J23" s="78">
         <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="K23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="28">
+      <c r="L23" s="28">
         <f>'NDBC NSTP6 timeseries data'!K465</f>
         <v>2.8666666666666667</v>
       </c>
-      <c r="K23" s="11">
+      <c r="M23" s="11">
         <f>'NDBC NSTP6 timeseries data'!L465</f>
         <v>253</v>
       </c>
-      <c r="L23" s="11">
+      <c r="N23" s="11">
         <f>'NDBC NSTP6 timeseries data'!M465</f>
         <v>11</v>
       </c>
-      <c r="M23" s="12" t="s">
+      <c r="O23" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N23" s="12"/>
-      <c r="O23" s="85" t="s">
+      <c r="P23" s="12"/>
+      <c r="Q23" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P23" s="92" t="s">
+      <c r="R23" s="89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="51">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="99">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C24" s="88">
+      <c r="D24" s="104">
+        <v>52</v>
+      </c>
+      <c r="E24" s="85">
         <v>41691</v>
       </c>
-      <c r="D24" s="11">
+      <c r="F24" s="11">
         <v>1040</v>
       </c>
-      <c r="E24" s="11">
+      <c r="G24" s="11">
         <v>1145</v>
       </c>
-      <c r="F24" s="11">
+      <c r="H24" s="11">
         <f>'NDBC NSTP6 timeseries data'!I467</f>
         <v>3.01</v>
       </c>
-      <c r="G24" s="11">
+      <c r="I24" s="11">
         <f>'NDBC NSTP6 timeseries data'!I479</f>
         <v>3.29</v>
       </c>
-      <c r="H24" s="81">
+      <c r="J24" s="78">
         <f t="shared" si="2"/>
         <v>0.28000000000000025</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J24" s="28">
+      <c r="L24" s="28">
         <f>'NDBC NSTP6 timeseries data'!K480</f>
         <v>3.8461538461538463</v>
       </c>
-      <c r="K24" s="27">
+      <c r="M24" s="27">
         <f>'NDBC NSTP6 timeseries data'!L480</f>
         <v>111.15384615384616</v>
       </c>
-      <c r="L24" s="11">
+      <c r="N24" s="11">
         <f>'NDBC NSTP6 timeseries data'!M480</f>
         <v>11</v>
       </c>
-      <c r="M24" s="12" t="s">
+      <c r="O24" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N24" s="12"/>
-      <c r="O24" s="85" t="s">
+      <c r="P24" s="12"/>
+      <c r="Q24" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P24" s="92" t="s">
+      <c r="R24" s="89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="78">
+        <v>135</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="100">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C25" s="89">
+      <c r="D25" s="104">
+        <v>52</v>
+      </c>
+      <c r="E25" s="86">
         <v>41691</v>
       </c>
-      <c r="D25" s="80">
+      <c r="F25" s="77">
         <v>1300</v>
       </c>
-      <c r="E25" s="80">
+      <c r="G25" s="77">
         <v>1400</v>
       </c>
-      <c r="F25" s="80">
+      <c r="H25" s="77">
         <f>'NDBC NSTP6 timeseries data'!I482</f>
         <v>3.24</v>
       </c>
-      <c r="G25" s="80">
+      <c r="I25" s="77">
         <f>'NDBC NSTP6 timeseries data'!I492</f>
         <v>2.97</v>
       </c>
-      <c r="H25" s="93">
+      <c r="J25" s="90">
         <f t="shared" si="2"/>
         <v>-0.27</v>
       </c>
-      <c r="I25" s="80" t="s">
+      <c r="K25" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="82">
+      <c r="L25" s="79">
         <f>'NDBC NSTP6 timeseries data'!K493</f>
         <v>3</v>
       </c>
-      <c r="K25" s="83">
+      <c r="M25" s="80">
         <f>'NDBC NSTP6 timeseries data'!L493</f>
         <v>193.45454545454547</v>
       </c>
-      <c r="L25" s="80">
+      <c r="N25" s="77">
         <f>'NDBC NSTP6 timeseries data'!M493</f>
         <v>16</v>
       </c>
-      <c r="M25" s="84" t="s">
+      <c r="O25" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="N25" s="84"/>
-      <c r="O25" s="85" t="s">
+      <c r="P25" s="81"/>
+      <c r="Q25" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="P25" s="92" t="s">
+      <c r="R25" s="89" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="95">
+        <v>135</v>
+      </c>
+      <c r="B26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="99">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="C26" s="94">
+      <c r="D26" s="104">
+        <v>52</v>
+      </c>
+      <c r="E26" s="85">
         <v>41691</v>
       </c>
-      <c r="D26" s="11">
+      <c r="F26" s="11">
         <v>1500</v>
       </c>
-      <c r="E26" s="11">
+      <c r="G26" s="11">
         <v>1550</v>
       </c>
-      <c r="F26" s="11">
+      <c r="H26" s="11">
         <f>'NDBC NSTP6 timeseries data'!I495</f>
         <v>2.39</v>
       </c>
-      <c r="G26" s="11">
+      <c r="I26" s="11">
         <f>'NDBC NSTP6 timeseries data'!I505</f>
         <v>1.86</v>
       </c>
-      <c r="H26" s="72">
+      <c r="J26" s="70">
         <f t="shared" si="2"/>
         <v>-0.53</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="K26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="28">
+      <c r="L26" s="28">
         <f>'NDBC NSTP6 timeseries data'!K506</f>
         <v>3.7272727272727271</v>
       </c>
-      <c r="K26" s="27">
+      <c r="M26" s="27">
         <f>'NDBC NSTP6 timeseries data'!L506</f>
         <v>152.27272727272728</v>
       </c>
-      <c r="L26" s="11">
+      <c r="N26" s="11">
         <f>'NDBC NSTP6 timeseries data'!M506</f>
         <v>11</v>
       </c>
-      <c r="M26" s="12" t="s">
+      <c r="O26" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12" t="s">
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P26" s="15" t="s">
+      <c r="R26" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" s="95">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="99">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C27" s="94">
+      <c r="D27" s="104">
+        <v>53</v>
+      </c>
+      <c r="E27" s="85">
         <v>41692</v>
       </c>
-      <c r="D27" s="11">
+      <c r="F27" s="11">
         <v>1100</v>
       </c>
-      <c r="E27" s="11">
+      <c r="G27" s="11">
         <v>1215</v>
       </c>
-      <c r="F27" s="11">
+      <c r="H27" s="11">
         <f>'NDBC NSTP6 timeseries data'!I508</f>
         <v>2.71</v>
       </c>
-      <c r="G27" s="11">
+      <c r="I27" s="11">
         <f>'NDBC NSTP6 timeseries data'!I521</f>
         <v>3.17</v>
       </c>
-      <c r="H27" s="32">
+      <c r="J27" s="32">
         <f t="shared" si="2"/>
         <v>0.45999999999999996</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="K27" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="11">
+      <c r="L27" s="11">
         <f>'NDBC NSTP6 timeseries data'!K522</f>
         <v>5.5</v>
       </c>
-      <c r="K27" s="27">
+      <c r="M27" s="27">
         <f>'NDBC NSTP6 timeseries data'!L522</f>
         <v>313.85714285714283</v>
       </c>
-      <c r="L27" s="11">
+      <c r="N27" s="11">
         <f>'NDBC NSTP6 timeseries data'!M522</f>
         <v>14</v>
       </c>
-      <c r="M27" s="12" t="s">
+      <c r="O27" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N27" s="11"/>
-      <c r="O27" s="12" t="s">
+      <c r="P27" s="11"/>
+      <c r="Q27" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P27" s="15" t="s">
+      <c r="R27" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28" s="95">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="99">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C28" s="94">
+      <c r="D28" s="104">
+        <v>53</v>
+      </c>
+      <c r="E28" s="85">
         <v>41692</v>
       </c>
-      <c r="D28" s="11">
+      <c r="F28" s="11">
         <v>1220</v>
       </c>
-      <c r="E28" s="11">
+      <c r="G28" s="11">
         <v>1315</v>
       </c>
-      <c r="F28" s="11">
+      <c r="H28" s="11">
         <f>'NDBC NSTP6 timeseries data'!I524</f>
         <v>3.19</v>
       </c>
-      <c r="G28" s="11">
+      <c r="I28" s="11">
         <f>'NDBC NSTP6 timeseries data'!I535</f>
         <v>3.37</v>
       </c>
-      <c r="H28" s="32">
+      <c r="J28" s="32">
         <f t="shared" si="2"/>
         <v>0.18000000000000016</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="K28" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J28" s="28">
+      <c r="L28" s="28">
         <f>'NDBC NSTP6 timeseries data'!K536</f>
         <v>6.333333333333333</v>
       </c>
-      <c r="K28" s="27">
+      <c r="M28" s="27">
         <f>'NDBC NSTP6 timeseries data'!L536</f>
         <v>301.5</v>
       </c>
-      <c r="L28" s="11">
+      <c r="N28" s="11">
         <f>'NDBC NSTP6 timeseries data'!M536</f>
         <v>12</v>
       </c>
-      <c r="M28" s="12" t="s">
+      <c r="O28" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N28" s="11"/>
-      <c r="O28" s="12" t="s">
+      <c r="P28" s="11"/>
+      <c r="Q28" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P28" s="15" t="s">
+      <c r="R28" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="95">
+        <v>127</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="99">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C29" s="94">
+      <c r="D29" s="104">
+        <v>53</v>
+      </c>
+      <c r="E29" s="85">
         <v>41692</v>
       </c>
-      <c r="D29" s="11">
+      <c r="F29" s="11">
         <v>1600</v>
       </c>
-      <c r="E29" s="11">
+      <c r="G29" s="11">
         <v>1700</v>
       </c>
-      <c r="F29" s="11">
+      <c r="H29" s="11">
         <f>'NDBC NSTP6 timeseries data'!I538</f>
         <v>2.44</v>
       </c>
-      <c r="G29" s="11">
+      <c r="I29" s="11">
         <f>'NDBC NSTP6 timeseries data'!I548</f>
         <v>1.92</v>
       </c>
-      <c r="H29" s="72">
+      <c r="J29" s="70">
         <f t="shared" si="2"/>
         <v>-0.52</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="K29" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="28">
+      <c r="L29" s="28">
         <f>'NDBC NSTP6 timeseries data'!K549</f>
         <v>4.1818181818181817</v>
       </c>
-      <c r="K29" s="27">
+      <c r="M29" s="27">
         <f>'NDBC NSTP6 timeseries data'!L549</f>
         <v>310.90909090909093</v>
       </c>
-      <c r="L29" s="11">
+      <c r="N29" s="11">
         <f>'NDBC NSTP6 timeseries data'!M549</f>
         <v>10</v>
       </c>
-      <c r="M29" s="12" t="s">
+      <c r="O29" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N29" s="11"/>
-      <c r="O29" s="12" t="s">
+      <c r="P29" s="11"/>
+      <c r="Q29" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P29" s="15" t="s">
+      <c r="R29" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" s="95">
+        <v>127</v>
+      </c>
+      <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="99">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="C30" s="94">
+      <c r="D30" s="104">
+        <v>53</v>
+      </c>
+      <c r="E30" s="85">
         <v>41692</v>
       </c>
-      <c r="D30" s="11">
+      <c r="F30" s="11">
         <v>1700</v>
       </c>
-      <c r="E30" s="11">
+      <c r="G30" s="11">
         <v>1845</v>
       </c>
-      <c r="F30" s="11">
+      <c r="H30" s="11">
         <f>'NDBC NSTP6 timeseries data'!I551</f>
         <v>1.92</v>
       </c>
-      <c r="G30" s="11">
+      <c r="I30" s="11">
         <f>'NDBC NSTP6 timeseries data'!I569</f>
         <v>1.21</v>
       </c>
-      <c r="H30" s="72">
+      <c r="J30" s="70">
         <f t="shared" si="2"/>
         <v>-0.71</v>
       </c>
-      <c r="I30" s="11" t="s">
+      <c r="K30" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="28">
+      <c r="L30" s="28">
         <f>'NDBC NSTP6 timeseries data'!K570</f>
         <v>2</v>
       </c>
-      <c r="K30" s="27">
+      <c r="M30" s="27">
         <f>'NDBC NSTP6 timeseries data'!L570</f>
         <v>242.47368421052633</v>
       </c>
-      <c r="L30" s="11">
+      <c r="N30" s="11">
         <f>'NDBC NSTP6 timeseries data'!M570</f>
         <v>10</v>
       </c>
-      <c r="M30" s="12" t="s">
+      <c r="O30" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="N30" s="11"/>
-      <c r="O30" s="12" t="s">
+      <c r="P30" s="11"/>
+      <c r="Q30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P30" s="15" t="s">
+      <c r="R30" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="95">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="99">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C31" s="94">
+      <c r="D31" s="104">
+        <v>54</v>
+      </c>
+      <c r="E31" s="85">
         <v>41693</v>
       </c>
-      <c r="D31" s="11">
+      <c r="F31" s="11">
         <v>1040</v>
       </c>
-      <c r="E31" s="11">
+      <c r="G31" s="11">
         <v>1210</v>
       </c>
-      <c r="F31" s="1">
+      <c r="H31" s="1">
         <f>'NDBC NSTP6 timeseries data'!I572</f>
         <v>2.0099999999999998</v>
       </c>
-      <c r="G31" s="1">
+      <c r="I31" s="1">
         <f>'NDBC NSTP6 timeseries data'!I587</f>
         <v>2.9</v>
       </c>
-      <c r="H31" s="72">
+      <c r="J31" s="70">
         <f t="shared" si="2"/>
         <v>0.89000000000000012</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="K31" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="28">
+      <c r="L31" s="28">
         <f>'NDBC NSTP6 timeseries data'!K588</f>
         <v>7.1875</v>
       </c>
-      <c r="K31" s="27">
+      <c r="M31" s="27">
         <f>'NDBC NSTP6 timeseries data'!L588</f>
         <v>304.1875</v>
       </c>
-      <c r="L31" s="11">
+      <c r="N31" s="11">
         <f>'NDBC NSTP6 timeseries data'!M588</f>
         <v>15</v>
       </c>
-      <c r="M31" s="12" t="s">
+      <c r="O31" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="N31" s="1"/>
-      <c r="O31" s="12" t="s">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P31" s="15" t="s">
+      <c r="R31" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="96">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="101">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="C32" s="97">
+      <c r="D32" s="105">
+        <v>54</v>
+      </c>
+      <c r="E32" s="102">
         <v>41693</v>
       </c>
-      <c r="D32" s="98">
+      <c r="F32" s="91">
         <v>1210</v>
       </c>
-      <c r="E32" s="98">
+      <c r="G32" s="91">
         <v>1255</v>
       </c>
-      <c r="F32" s="16">
+      <c r="H32" s="16">
         <f>'NDBC NSTP6 timeseries data'!I590</f>
         <v>2.9</v>
       </c>
-      <c r="G32" s="16">
+      <c r="I32" s="16">
         <f>'NDBC NSTP6 timeseries data'!I599</f>
         <v>3.27</v>
       </c>
-      <c r="H32" s="99">
+      <c r="J32" s="92">
         <f t="shared" si="2"/>
         <v>0.37000000000000011</v>
       </c>
-      <c r="I32" s="98" t="s">
+      <c r="K32" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="100">
+      <c r="L32" s="93">
         <f>'NDBC NSTP6 timeseries data'!K600</f>
         <v>5.2857142857142856</v>
       </c>
-      <c r="K32" s="101">
+      <c r="M32" s="94">
         <f>'NDBC NSTP6 timeseries data'!L600</f>
         <v>260.28571428571428</v>
       </c>
-      <c r="L32" s="98">
+      <c r="N32" s="91">
         <f>'NDBC NSTP6 timeseries data'!M600</f>
         <v>11</v>
       </c>
-      <c r="M32" s="102" t="s">
+      <c r="O32" s="95" t="s">
         <v>100</v>
       </c>
-      <c r="N32" s="16"/>
-      <c r="O32" s="102" t="s">
+      <c r="P32" s="16"/>
+      <c r="Q32" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="P32" s="103" t="s">
+      <c r="R32" s="96" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L3:L16">
+  <conditionalFormatting sqref="N3:N16">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1"/>
-    <hyperlink ref="J1:K1" r:id="rId2" display="NSTP6"/>
-    <hyperlink ref="L1" r:id="rId3" display="NSTP6"/>
+    <hyperlink ref="H1" r:id="rId1"/>
+    <hyperlink ref="L1:M1" r:id="rId2" display="NSTP6"/>
+    <hyperlink ref="N1" r:id="rId3" display="NSTP6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
@@ -3831,24 +3994,24 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="21"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52" t="s">
         <v>95</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="53" t="s">
         <v>96</v>
       </c>
       <c r="B3" s="41"/>
@@ -3870,13 +4033,13 @@
       <c r="J3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="54" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -3885,17 +4048,17 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="59"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="60"/>
+      <c r="K4" s="58"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="4" t="s">
         <v>53</v>
       </c>
@@ -3904,7 +4067,7 @@
       <c r="F5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="59"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="4" t="s">
         <v>53</v>
       </c>
@@ -3912,32 +4075,32 @@
       <c r="J5" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="60" t="s">
+      <c r="K5" s="58" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63" t="s">
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64" t="s">
+      <c r="D6" s="62"/>
+      <c r="E6" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="65"/>
-      <c r="H6" s="63" t="s">
+      <c r="G6" s="63"/>
+      <c r="H6" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="64"/>
+      <c r="I6" s="62"/>
       <c r="J6" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="K6" s="66" t="s">
+      <c r="K6" s="64" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3953,27 +4116,27 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="54" t="s">
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="J8" s="69"/>
-      <c r="K8" s="70"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="68"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="58"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
         <v>57</v>
@@ -3984,7 +4147,7 @@
       <c r="F9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="59"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
         <v>57</v>
@@ -3992,13 +4155,13 @@
       <c r="J9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="54" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58" t="s">
+      <c r="A10" s="55"/>
+      <c r="B10" s="56" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -4007,17 +4170,17 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="59"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="60"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="4" t="s">
         <v>53</v>
       </c>
@@ -4026,38 +4189,38 @@
       <c r="F11" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="59"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="58" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="61"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="63" t="s">
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64" t="s">
+      <c r="D12" s="62"/>
+      <c r="E12" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="65"/>
-      <c r="H12" s="63" t="s">
+      <c r="G12" s="63"/>
+      <c r="H12" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64" t="s">
+      <c r="I12" s="62"/>
+      <c r="J12" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="K12" s="71" t="s">
+      <c r="K12" s="69" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4066,7 +4229,7 @@
         <v>121</v>
       </c>
       <c r="E14">
-        <f>COUNTIF(Table!I3:I32,"rising")</f>
+        <f>COUNTIF(Table!K3:K32,"rising")</f>
         <v>14</v>
       </c>
     </row>
@@ -4075,27 +4238,27 @@
         <v>122</v>
       </c>
       <c r="E15">
-        <f>COUNTIF(Table!I3:I32,"falling")</f>
+        <f>COUNTIF(Table!K3:K32,"falling")</f>
         <v>15</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -4180,11 +4343,11 @@
       <c r="A1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -4963,11 +5126,11 @@
         <f>I24-I4</f>
         <v>-0.56499999999999995</v>
       </c>
-      <c r="K25" s="52">
+      <c r="K25" s="50">
         <f>AVERAGE(K4:K24)</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="L25" s="52">
+      <c r="L25" s="50">
         <f>AVERAGE(L4:L24)</f>
         <v>232.5</v>
       </c>
@@ -5700,11 +5863,11 @@
         <f>I42-I27</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="K43" s="52">
+      <c r="K43" s="50">
         <f>AVERAGE(K27:K42)</f>
         <v>2.375</v>
       </c>
-      <c r="L43" s="52">
+      <c r="L43" s="50">
         <f>AVERAGE(L27:L42)</f>
         <v>193.6875</v>
       </c>
@@ -6437,11 +6600,11 @@
         <f>I60-I45</f>
         <v>0.71</v>
       </c>
-      <c r="K61" s="52">
+      <c r="K61" s="50">
         <f>AVERAGE(K45:K60)</f>
         <v>3.25</v>
       </c>
-      <c r="L61" s="52">
+      <c r="L61" s="50">
         <f>AVERAGE(L45:L60)</f>
         <v>258.375</v>
       </c>
@@ -7201,11 +7364,11 @@
         <v>-1.161</v>
       </c>
       <c r="J84" s="5"/>
-      <c r="K84" s="52">
+      <c r="K84" s="50">
         <f>AVERAGE(K68:K83)</f>
         <v>5.2725</v>
       </c>
-      <c r="L84" s="52">
+      <c r="L84" s="50">
         <f>AVERAGE(L68:L83)</f>
         <v>96.1875</v>
       </c>
@@ -7940,11 +8103,11 @@
         <v>-1.35</v>
       </c>
       <c r="J102" s="5"/>
-      <c r="K102" s="52">
+      <c r="K102" s="50">
         <f>AVERAGE(K86:K101)</f>
         <v>5.6875</v>
       </c>
-      <c r="L102" s="52">
+      <c r="L102" s="50">
         <f>AVERAGE(L86:L101)</f>
         <v>100.25</v>
       </c>
@@ -8896,11 +9059,11 @@
         <v>1.7100000000000002</v>
       </c>
       <c r="J125" s="5"/>
-      <c r="K125" s="52">
+      <c r="K125" s="50">
         <f>AVERAGE(K104:K124)</f>
         <v>4.2380952380952381</v>
       </c>
-      <c r="L125" s="52">
+      <c r="L125" s="50">
         <f>AVERAGE(L104:L124)</f>
         <v>187.95238095238096</v>
       </c>
@@ -9679,11 +9842,11 @@
         <v>0.35000000000000009</v>
       </c>
       <c r="J144" s="5"/>
-      <c r="K144" s="52">
+      <c r="K144" s="50">
         <f>AVERAGE(K127:K143)</f>
         <v>5.2352941176470589</v>
       </c>
-      <c r="L144" s="52">
+      <c r="L144" s="50">
         <f>AVERAGE(L127:L143)</f>
         <v>140.41176470588235</v>
       </c>
@@ -10673,11 +10836,11 @@
         <v>-0.80000000000000027</v>
       </c>
       <c r="J168" s="5"/>
-      <c r="K168" s="52">
+      <c r="K168" s="50">
         <f>AVERAGE(K146:K167)</f>
         <v>6.0454545454545459</v>
       </c>
-      <c r="L168" s="52">
+      <c r="L168" s="50">
         <f>AVERAGE(L146:L167)</f>
         <v>144.13636363636363</v>
       </c>
@@ -11580,11 +11743,11 @@
         <v>0.85999999999999988</v>
       </c>
       <c r="J190" s="5"/>
-      <c r="K190" s="52">
+      <c r="K190" s="50">
         <f>AVERAGE(K170:K189)</f>
         <v>3.25</v>
       </c>
-      <c r="L190" s="52">
+      <c r="L190" s="50">
         <f>AVERAGE(L170:L189)</f>
         <v>168.8</v>
       </c>
@@ -12662,11 +12825,11 @@
         <v>-0.51</v>
       </c>
       <c r="J216" s="5"/>
-      <c r="K216" s="52">
+      <c r="K216" s="50">
         <f>AVERAGE(K192:K215)</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="L216" s="52">
+      <c r="L216" s="50">
         <f>AVERAGE(L192:L215)</f>
         <v>79.958333333333329</v>
       </c>
@@ -13528,11 +13691,11 @@
         <v>0.45000000000000018</v>
       </c>
       <c r="J237" s="5"/>
-      <c r="K237" s="52">
+      <c r="K237" s="50">
         <f>AVERAGE(K218:K236)</f>
         <v>5.8947368421052628</v>
       </c>
-      <c r="L237" s="52">
+      <c r="L237" s="50">
         <f>AVERAGE(L218:L236)</f>
         <v>101.36842105263158</v>
       </c>
@@ -14350,11 +14513,11 @@
         <v>0.94</v>
       </c>
       <c r="J257" s="5"/>
-      <c r="K257" s="52">
+      <c r="K257" s="50">
         <f>AVERAGE(K239:K256)</f>
         <v>5.166666666666667</v>
       </c>
-      <c r="L257" s="52">
+      <c r="L257" s="50">
         <f>AVERAGE(L239:L256)</f>
         <v>89.888888888888886</v>
       </c>
@@ -15344,11 +15507,11 @@
         <v>-0.82999999999999985</v>
       </c>
       <c r="J281" s="5"/>
-      <c r="K281" s="52">
+      <c r="K281" s="50">
         <f>AVERAGE(K259:K280)</f>
         <v>4.9090909090909092</v>
       </c>
-      <c r="L281" s="52">
+      <c r="L281" s="50">
         <f>AVERAGE(L259:L280)</f>
         <v>97.727272727272734</v>
       </c>
@@ -16426,11 +16589,11 @@
         <v>7.0000000000000062E-2</v>
       </c>
       <c r="J307" s="5"/>
-      <c r="K307" s="52">
+      <c r="K307" s="50">
         <f>AVERAGE(K283:K306)</f>
         <v>4.708333333333333</v>
       </c>
-      <c r="L307" s="52">
+      <c r="L307" s="50">
         <f>AVERAGE(L283:L306)</f>
         <v>194.41666666666666</v>
       </c>
@@ -17488,11 +17651,11 @@
         <v>-1.3649999999999998</v>
       </c>
       <c r="J337" s="5"/>
-      <c r="K337" s="52">
+      <c r="K337" s="50">
         <f>AVERAGE(K309:K336)</f>
         <v>5.7757142857142858</v>
       </c>
-      <c r="L337" s="52">
+      <c r="L337" s="50">
         <f>AVERAGE(L309:L336)</f>
         <v>39.857142857142854</v>
       </c>
@@ -18567,11 +18730,11 @@
         <v>-0.27600000000000002</v>
       </c>
       <c r="J366" s="5"/>
-      <c r="K366" s="52">
+      <c r="K366" s="50">
         <f>AVERAGE(K339:K365)</f>
         <v>6.565555555555556</v>
       </c>
-      <c r="L366" s="52">
+      <c r="L366" s="50">
         <f>AVERAGE(L339:L365)</f>
         <v>54.407407407407405</v>
       </c>
@@ -19561,11 +19724,11 @@
         <v>0.62999999999999989</v>
       </c>
       <c r="J390" s="5"/>
-      <c r="K390" s="52">
+      <c r="K390" s="50">
         <f>AVERAGE(K368:K389)</f>
         <v>4.8181818181818183</v>
       </c>
-      <c r="L390" s="52">
+      <c r="L390" s="50">
         <f>AVERAGE(L368:L389)</f>
         <v>290.22727272727275</v>
       </c>
@@ -20071,11 +20234,11 @@
         <v>-0.15000000000000036</v>
       </c>
       <c r="J403" s="5"/>
-      <c r="K403" s="52">
+      <c r="K403" s="50">
         <f>AVERAGE(K392:K402)</f>
         <v>4.2727272727272725</v>
       </c>
-      <c r="L403" s="52">
+      <c r="L403" s="50">
         <f>AVERAGE(L392:L402)</f>
         <v>117.18181818181819</v>
       </c>
@@ -21197,11 +21360,11 @@
         <v>-0.96</v>
       </c>
       <c r="J430" s="5"/>
-      <c r="K430" s="52">
+      <c r="K430" s="50">
         <f>AVERAGE(K405:K429)</f>
         <v>2.96</v>
       </c>
-      <c r="L430" s="52">
+      <c r="L430" s="50">
         <f>AVERAGE(L405:L429)</f>
         <v>237.8</v>
       </c>
@@ -21927,11 +22090,11 @@
         <v>-0.56000000000000005</v>
       </c>
       <c r="J448" s="5"/>
-      <c r="K448" s="52">
+      <c r="K448" s="50">
         <f>AVERAGE(K432:K447)</f>
         <v>5.9375</v>
       </c>
-      <c r="L448" s="52">
+      <c r="L448" s="50">
         <f>AVERAGE(L432:L447)</f>
         <v>290</v>
       </c>
@@ -22613,11 +22776,11 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="J465" s="5"/>
-      <c r="K465" s="52">
+      <c r="K465" s="50">
         <f>AVERAGE(K450:K464)</f>
         <v>2.8666666666666667</v>
       </c>
-      <c r="L465" s="52">
+      <c r="L465" s="50">
         <f>AVERAGE(L456:L464)</f>
         <v>253</v>
       </c>
@@ -23211,11 +23374,11 @@
         <v>0.28000000000000025</v>
       </c>
       <c r="J480" s="5"/>
-      <c r="K480" s="52">
+      <c r="K480" s="50">
         <f>AVERAGE(K467:K479)</f>
         <v>3.8461538461538463</v>
       </c>
-      <c r="L480" s="52">
+      <c r="L480" s="50">
         <f>AVERAGE(L467:L479)</f>
         <v>111.15384615384616</v>
       </c>
@@ -23721,11 +23884,11 @@
         <v>-0.27</v>
       </c>
       <c r="J493" s="5"/>
-      <c r="K493" s="52">
+      <c r="K493" s="50">
         <f>AVERAGE(K482:K492)</f>
         <v>3</v>
       </c>
-      <c r="L493" s="52">
+      <c r="L493" s="50">
         <f>AVERAGE(L482:L492)</f>
         <v>193.45454545454547</v>
       </c>
@@ -24231,11 +24394,11 @@
         <v>-0.53</v>
       </c>
       <c r="J506" s="5"/>
-      <c r="K506" s="52">
+      <c r="K506" s="50">
         <f>AVERAGE(K495:K505)</f>
         <v>3.7272727272727271</v>
       </c>
-      <c r="L506" s="52">
+      <c r="L506" s="50">
         <f>AVERAGE(L495:L505)</f>
         <v>152.27272727272728</v>
       </c>
@@ -24873,11 +25036,11 @@
         <v>0.45999999999999996</v>
       </c>
       <c r="J522" s="5"/>
-      <c r="K522" s="52">
+      <c r="K522" s="50">
         <f>AVERAGE(K508:K521)</f>
         <v>5.5</v>
       </c>
-      <c r="L522" s="52">
+      <c r="L522" s="50">
         <f>AVERAGE(L508:L521)</f>
         <v>313.85714285714283</v>
       </c>
@@ -25427,11 +25590,11 @@
         <v>0.18000000000000016</v>
       </c>
       <c r="J536" s="5"/>
-      <c r="K536" s="52">
+      <c r="K536" s="50">
         <f>AVERAGE(K524:K535)</f>
         <v>6.333333333333333</v>
       </c>
-      <c r="L536" s="52">
+      <c r="L536" s="50">
         <f>AVERAGE(L524:L535)</f>
         <v>301.5</v>
       </c>
@@ -25937,11 +26100,11 @@
         <v>-0.52</v>
       </c>
       <c r="J549" s="5"/>
-      <c r="K549" s="52">
+      <c r="K549" s="50">
         <f>AVERAGE(K538:K548)</f>
         <v>4.1818181818181817</v>
       </c>
-      <c r="L549" s="52">
+      <c r="L549" s="50">
         <f>AVERAGE(L538:L548)</f>
         <v>310.90909090909093</v>
       </c>
@@ -26799,11 +26962,11 @@
         <v>-0.71</v>
       </c>
       <c r="J570" s="5"/>
-      <c r="K570" s="52">
+      <c r="K570" s="50">
         <f>AVERAGE(K551:K569)</f>
         <v>2</v>
       </c>
-      <c r="L570" s="52">
+      <c r="L570" s="50">
         <f>AVERAGE(L551:L569)</f>
         <v>242.47368421052633</v>
       </c>
@@ -27529,11 +27692,11 @@
         <v>0.89000000000000012</v>
       </c>
       <c r="J588" s="5"/>
-      <c r="K588" s="52">
+      <c r="K588" s="50">
         <f>AVERAGE(K572:K587)</f>
         <v>7.1875</v>
       </c>
-      <c r="L588" s="52">
+      <c r="L588" s="50">
         <f>AVERAGE(L572:L587)</f>
         <v>304.1875</v>
       </c>
@@ -27995,11 +28158,11 @@
         <v>0.37000000000000011</v>
       </c>
       <c r="J600" s="5"/>
-      <c r="K600" s="52">
+      <c r="K600" s="50">
         <f>AVERAGE(K593:K599)</f>
         <v>5.2857142857142856</v>
       </c>
-      <c r="L600" s="52">
+      <c r="L600" s="50">
         <f>AVERAGE(L593:L599)</f>
         <v>260.28571428571428</v>
       </c>
@@ -28052,13 +28215,13 @@
       <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">

</xml_diff>

<commit_message>
set up manuscript python docx
</commit_message>
<xml_diff>
--- a/Data/Drifter deployment checklist.xlsx
+++ b/Data/Drifter deployment checklist.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
-    <sheet name="Matrix" sheetId="1" r:id="rId2"/>
-    <sheet name="NDBC NSTP6 timeseries data" sheetId="5" r:id="rId3"/>
-    <sheet name="NDBC NSTP6 data UTC no water le" sheetId="3" r:id="rId4"/>
+    <sheet name="EndmemberDefn" sheetId="6" r:id="rId2"/>
+    <sheet name="Matrix" sheetId="1" r:id="rId3"/>
+    <sheet name="NDBC NSTP6 timeseries data" sheetId="5" r:id="rId4"/>
+    <sheet name="NDBC NSTP6 data UTC no water le" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="150">
   <si>
     <t>Swell</t>
   </si>
@@ -436,6 +437,48 @@
   <si>
     <t>tide</t>
   </si>
+  <si>
+    <t>End member</t>
+  </si>
+  <si>
+    <t>Julian Day</t>
+  </si>
+  <si>
+    <t>Gregorian Day (UTC)</t>
+  </si>
+  <si>
+    <t>Gregorian Day (Local)</t>
+  </si>
+  <si>
+    <t>Tide/Calm</t>
+  </si>
+  <si>
+    <t>50-51</t>
+  </si>
+  <si>
+    <t>2/19-2/20</t>
+  </si>
+  <si>
+    <t>2/18-2/19</t>
+  </si>
+  <si>
+    <t>47-49</t>
+  </si>
+  <si>
+    <t>2/16-2/18</t>
+  </si>
+  <si>
+    <t>2/15-2/17</t>
+  </si>
+  <si>
+    <t>52-55</t>
+  </si>
+  <si>
+    <t>2/21-2/24</t>
+  </si>
+  <si>
+    <t>2/20-2/23</t>
+  </si>
 </sst>
 </file>
 
@@ -533,7 +576,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -912,12 +955,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1157,9 +1237,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1183,6 +1260,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2021,18 +2113,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="4" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
@@ -2082,7 +2175,7 @@
       <c r="C2" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="103" t="s">
+      <c r="D2" s="102" t="s">
         <v>131</v>
       </c>
       <c r="E2" s="83" t="s">
@@ -2132,10 +2225,10 @@
       <c r="A3" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="98">
+      <c r="C3" s="97">
         <v>1</v>
       </c>
-      <c r="D3" s="104">
+      <c r="D3" s="103">
         <v>19</v>
       </c>
       <c r="E3" s="84">
@@ -2189,11 +2282,11 @@
       <c r="A4" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="99">
+      <c r="C4" s="98">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="D4" s="104">
+      <c r="D4" s="103">
         <v>20</v>
       </c>
       <c r="E4" s="85">
@@ -2247,11 +2340,11 @@
       <c r="A5" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="99">
+      <c r="C5" s="98">
         <f>C4+1</f>
         <v>3</v>
       </c>
-      <c r="D5" s="104">
+      <c r="D5" s="103">
         <v>20</v>
       </c>
       <c r="E5" s="85">
@@ -2305,11 +2398,11 @@
       <c r="A6" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="99">
+      <c r="C6" s="98">
         <f t="shared" ref="C6:C32" si="1">C5+1</f>
         <v>4</v>
       </c>
-      <c r="D6" s="104">
+      <c r="D6" s="103">
         <v>32</v>
       </c>
       <c r="E6" s="85">
@@ -2361,11 +2454,11 @@
       <c r="A7" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="98">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="D7" s="104">
+      <c r="D7" s="103">
         <v>32</v>
       </c>
       <c r="E7" s="85">
@@ -2417,11 +2510,11 @@
       <c r="A8" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="99">
+      <c r="C8" s="98">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="D8" s="104">
+      <c r="D8" s="103">
         <v>32</v>
       </c>
       <c r="E8" s="85">
@@ -2473,11 +2566,11 @@
       <c r="A9" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="99">
+      <c r="C9" s="98">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="D9" s="104">
+      <c r="D9" s="103">
         <v>39</v>
       </c>
       <c r="E9" s="85">
@@ -2534,11 +2627,11 @@
       <c r="A10" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="99">
+      <c r="C10" s="98">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D10" s="104">
+      <c r="D10" s="103">
         <v>39</v>
       </c>
       <c r="E10" s="85">
@@ -2598,11 +2691,11 @@
       <c r="B11" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="99">
+      <c r="C11" s="98">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D11" s="104">
+      <c r="D11" s="103">
         <v>47</v>
       </c>
       <c r="E11" s="85">
@@ -2662,11 +2755,11 @@
       <c r="B12" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="99">
+      <c r="C12" s="98">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D12" s="104">
+      <c r="D12" s="103">
         <v>48</v>
       </c>
       <c r="E12" s="85">
@@ -2726,11 +2819,11 @@
       <c r="B13" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="99">
+      <c r="C13" s="98">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D13" s="104">
+      <c r="D13" s="103">
         <v>48</v>
       </c>
       <c r="E13" s="85">
@@ -2790,11 +2883,11 @@
       <c r="B14" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="99">
+      <c r="C14" s="98">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D14" s="104">
+      <c r="D14" s="103">
         <v>48</v>
       </c>
       <c r="E14" s="85">
@@ -2854,11 +2947,11 @@
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="99">
+      <c r="C15" s="98">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="D15" s="104">
+      <c r="D15" s="103">
         <v>49</v>
       </c>
       <c r="E15" s="85">
@@ -2918,11 +3011,11 @@
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="100">
+      <c r="C16" s="99">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="D16" s="104">
+      <c r="D16" s="103">
         <v>49</v>
       </c>
       <c r="E16" s="86">
@@ -2982,11 +3075,11 @@
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="99">
+      <c r="C17" s="98">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="D17" s="104">
+      <c r="D17" s="103">
         <v>50</v>
       </c>
       <c r="E17" s="85">
@@ -3043,11 +3136,11 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="99">
+      <c r="C18" s="98">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="D18" s="104">
+      <c r="D18" s="103">
         <v>50</v>
       </c>
       <c r="E18" s="85">
@@ -3104,11 +3197,11 @@
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="99">
+      <c r="C19" s="98">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="D19" s="104">
+      <c r="D19" s="103">
         <v>51</v>
       </c>
       <c r="E19" s="85">
@@ -3165,11 +3258,11 @@
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="99">
+      <c r="C20" s="98">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="D20" s="104">
+      <c r="D20" s="103">
         <v>51</v>
       </c>
       <c r="E20" s="85">
@@ -3226,11 +3319,11 @@
       <c r="B21" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="99">
+      <c r="C21" s="98">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D21" s="104">
+      <c r="D21" s="103">
         <v>51</v>
       </c>
       <c r="E21" s="85">
@@ -3287,11 +3380,11 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="99">
+      <c r="C22" s="98">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="D22" s="104">
+      <c r="D22" s="103">
         <v>51</v>
       </c>
       <c r="E22" s="85">
@@ -3348,11 +3441,11 @@
       <c r="B23" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="99">
+      <c r="C23" s="98">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="D23" s="104">
+      <c r="D23" s="103">
         <v>52</v>
       </c>
       <c r="E23" s="85">
@@ -3409,11 +3502,11 @@
       <c r="B24" t="s">
         <v>134</v>
       </c>
-      <c r="C24" s="99">
+      <c r="C24" s="98">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="D24" s="104">
+      <c r="D24" s="103">
         <v>52</v>
       </c>
       <c r="E24" s="85">
@@ -3470,11 +3563,11 @@
       <c r="B25" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="100">
+      <c r="C25" s="99">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="D25" s="104">
+      <c r="D25" s="103">
         <v>52</v>
       </c>
       <c r="E25" s="86">
@@ -3531,11 +3624,11 @@
       <c r="B26" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="99">
+      <c r="C26" s="98">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="D26" s="104">
+      <c r="D26" s="103">
         <v>52</v>
       </c>
       <c r="E26" s="85">
@@ -3592,11 +3685,11 @@
       <c r="B27" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="99">
+      <c r="C27" s="98">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="D27" s="104">
+      <c r="D27" s="103">
         <v>53</v>
       </c>
       <c r="E27" s="85">
@@ -3653,11 +3746,11 @@
       <c r="B28" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="99">
+      <c r="C28" s="98">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="D28" s="104">
+      <c r="D28" s="103">
         <v>53</v>
       </c>
       <c r="E28" s="85">
@@ -3714,11 +3807,11 @@
       <c r="B29" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="99">
+      <c r="C29" s="98">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="D29" s="104">
+      <c r="D29" s="103">
         <v>53</v>
       </c>
       <c r="E29" s="85">
@@ -3775,11 +3868,11 @@
       <c r="B30" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="99">
+      <c r="C30" s="98">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="D30" s="104">
+      <c r="D30" s="103">
         <v>53</v>
       </c>
       <c r="E30" s="85">
@@ -3836,11 +3929,11 @@
       <c r="B31" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="99">
+      <c r="C31" s="98">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="D31" s="104">
+      <c r="D31" s="103">
         <v>54</v>
       </c>
       <c r="E31" s="85">
@@ -3897,14 +3990,14 @@
       <c r="B32" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="101">
+      <c r="C32" s="100">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="D32" s="105">
+      <c r="D32" s="104">
         <v>54</v>
       </c>
-      <c r="E32" s="102">
+      <c r="E32" s="101">
         <v>41693</v>
       </c>
       <c r="F32" s="91">
@@ -3968,6 +4061,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="106" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="107" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="107" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="108" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="108" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="109" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="109" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="109" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="108" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="109" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="109" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="109" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
@@ -4311,7 +4479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y600"/>
   <sheetViews>
@@ -4343,11 +4511,11 @@
       <c r="A1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -28184,7 +28352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z61"/>
   <sheetViews>
@@ -28215,13 +28383,13 @@
       <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">

</xml_diff>

<commit_message>
Changes to figures and tables
Curt's suggestions on maps, figures, and tables
</commit_message>
<xml_diff>
--- a/Data/Drifter deployment checklist.xlsx
+++ b/Data/Drifter deployment checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
@@ -423,9 +423,6 @@
     <t>*only drifters D1,D3,D4,D5-D1 has some weird issue in the middle of it</t>
   </si>
   <si>
-    <t>Julian(local)</t>
-  </si>
-  <si>
     <t>EndMember</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
   </si>
   <si>
     <t>End member</t>
-  </si>
-  <si>
-    <t>Julian Day</t>
   </si>
   <si>
     <t>Gregorian Day (UTC)</t>
@@ -478,6 +472,12 @@
   </si>
   <si>
     <t>2/20-2/23</t>
+  </si>
+  <si>
+    <t>Year Day 2014</t>
+  </si>
+  <si>
+    <t>Year Day 2014 (local)</t>
   </si>
 </sst>
 </file>
@@ -1261,9 +1261,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1275,6 +1272,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2113,11 +2113,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,13 +2170,13 @@
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="87" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="102" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="E2" s="83" t="s">
         <v>1</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="97">
         <v>1</v>
@@ -2280,7 +2280,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" s="98">
         <f>C3+1</f>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="98">
         <f>C4+1</f>
@@ -2686,10 +2686,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" s="98">
         <f t="shared" si="1"/>
@@ -2753,7 +2753,7 @@
         <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="98">
         <f t="shared" si="1"/>
@@ -2817,7 +2817,7 @@
         <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C13" s="98">
         <f t="shared" si="1"/>
@@ -2881,7 +2881,7 @@
         <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="98">
         <f t="shared" si="1"/>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -3436,10 +3436,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C23" s="98">
         <f t="shared" si="1"/>
@@ -3497,10 +3497,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="98">
         <f t="shared" si="1"/>
@@ -3558,10 +3558,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C25" s="99">
         <f t="shared" si="1"/>
@@ -3619,10 +3619,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" s="98">
         <f t="shared" si="1"/>
@@ -3683,7 +3683,7 @@
         <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="98">
         <f t="shared" si="1"/>
@@ -3744,7 +3744,7 @@
         <v>127</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" s="98">
         <f t="shared" si="1"/>
@@ -3805,7 +3805,7 @@
         <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" s="98">
         <f t="shared" si="1"/>
@@ -3866,7 +3866,7 @@
         <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C30" s="98">
         <f t="shared" si="1"/>
@@ -3927,7 +3927,7 @@
         <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C31" s="98">
         <f t="shared" si="1"/>
@@ -3988,7 +3988,7 @@
         <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C32" s="100">
         <f t="shared" si="1"/>
@@ -4064,8 +4064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4073,60 +4073,60 @@
     <col min="1" max="4" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="106" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="D1" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="107" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="108" t="s">
+      <c r="C2" s="108" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="D2" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="109" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="107" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="108" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="109" t="s">
+      <c r="C3" s="108" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108" t="s">
+      <c r="D3" s="108" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="109" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="109" t="s">
+      <c r="B4" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="C4" s="108" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="108" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="109" t="s">
+      <c r="D4" s="108" t="s">
         <v>147</v>
-      </c>
-      <c r="C4" s="109" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="109" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4511,11 +4511,11 @@
       <c r="A1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -28383,13 +28383,13 @@
       <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="105" t="s">
+      <c r="H1" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">

</xml_diff>

<commit_message>
Revised Draft and off to Curt
</commit_message>
<xml_diff>
--- a/Data/Drifter deployment checklist.xlsx
+++ b/Data/Drifter deployment checklist.xlsx
@@ -1304,9 +1304,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1317,6 +1314,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2157,10 +2157,10 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="L9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P36" sqref="P36"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,8 +2173,9 @@
     <col min="6" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" customWidth="1"/>
-    <col min="12" max="13" width="16.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" customWidth="1"/>
     <col min="15" max="16" width="14.5703125" customWidth="1"/>
     <col min="17" max="17" width="8" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" customWidth="1"/>
@@ -2317,7 +2318,7 @@
       <c r="O3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="113" t="s">
+      <c r="P3" s="112" t="s">
         <v>154</v>
       </c>
       <c r="Q3" s="13"/>
@@ -2381,7 +2382,7 @@
       <c r="P4" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="Q4" s="110"/>
+      <c r="Q4" s="109"/>
       <c r="R4" s="75" t="s">
         <v>11</v>
       </c>
@@ -2442,7 +2443,7 @@
       <c r="P5" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="Q5" s="110"/>
+      <c r="Q5" s="109"/>
       <c r="R5" s="75" t="s">
         <v>11</v>
       </c>
@@ -2501,7 +2502,7 @@
       <c r="P6" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="Q6" s="110"/>
+      <c r="Q6" s="109"/>
       <c r="R6" s="75" t="s">
         <v>10</v>
       </c>
@@ -2560,7 +2561,7 @@
       <c r="P7" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="Q7" s="110"/>
+      <c r="Q7" s="109"/>
       <c r="R7" s="75" t="s">
         <v>11</v>
       </c>
@@ -2619,7 +2620,7 @@
       <c r="P8" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="Q8" s="110"/>
+      <c r="Q8" s="109"/>
       <c r="R8" s="75" t="s">
         <v>10</v>
       </c>
@@ -2680,7 +2681,7 @@
       <c r="P9" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q9" s="110"/>
+      <c r="Q9" s="109"/>
       <c r="R9" s="75" t="s">
         <v>11</v>
       </c>
@@ -2744,7 +2745,7 @@
       <c r="P10" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q10" s="110"/>
+      <c r="Q10" s="109"/>
       <c r="R10" s="75" t="s">
         <v>11</v>
       </c>
@@ -2811,7 +2812,7 @@
       <c r="P11" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="Q11" s="110"/>
+      <c r="Q11" s="109"/>
       <c r="R11" s="75" t="s">
         <v>11</v>
       </c>
@@ -2878,7 +2879,7 @@
       <c r="P12" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q12" s="110"/>
+      <c r="Q12" s="109"/>
       <c r="R12" s="75" t="s">
         <v>10</v>
       </c>
@@ -2945,7 +2946,7 @@
       <c r="P13" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q13" s="110"/>
+      <c r="Q13" s="109"/>
       <c r="R13" s="75" t="s">
         <v>11</v>
       </c>
@@ -3012,7 +3013,7 @@
       <c r="P14" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q14" s="110"/>
+      <c r="Q14" s="109"/>
       <c r="R14" s="75" t="s">
         <v>11</v>
       </c>
@@ -3079,7 +3080,7 @@
       <c r="P15" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q15" s="110"/>
+      <c r="Q15" s="109"/>
       <c r="R15" s="75" t="s">
         <v>10</v>
       </c>
@@ -3146,7 +3147,7 @@
       <c r="P16" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q16" s="111"/>
+      <c r="Q16" s="110"/>
       <c r="R16" s="82" t="s">
         <v>10</v>
       </c>
@@ -3213,7 +3214,7 @@
       <c r="P17" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q17" s="110"/>
+      <c r="Q17" s="109"/>
       <c r="R17" s="82" t="s">
         <v>10</v>
       </c>
@@ -3277,7 +3278,7 @@
       <c r="P18" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q18" s="110"/>
+      <c r="Q18" s="109"/>
       <c r="R18" s="75" t="s">
         <v>11</v>
       </c>
@@ -3341,7 +3342,7 @@
       <c r="P19" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="Q19" s="110"/>
+      <c r="Q19" s="109"/>
       <c r="R19" s="82" t="s">
         <v>10</v>
       </c>
@@ -3405,7 +3406,7 @@
       <c r="P20" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="Q20" s="110"/>
+      <c r="Q20" s="109"/>
       <c r="R20" s="82" t="s">
         <v>10</v>
       </c>
@@ -3469,7 +3470,7 @@
       <c r="P21" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="Q21" s="110"/>
+      <c r="Q21" s="109"/>
       <c r="R21" s="75" t="s">
         <v>11</v>
       </c>
@@ -3533,7 +3534,7 @@
       <c r="P22" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="Q22" s="110"/>
+      <c r="Q22" s="109"/>
       <c r="R22" s="75" t="s">
         <v>11</v>
       </c>
@@ -3597,7 +3598,7 @@
       <c r="P23" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="Q23" s="112"/>
+      <c r="Q23" s="111"/>
       <c r="R23" s="82" t="s">
         <v>10</v>
       </c>
@@ -4648,11 +4649,11 @@
       <c r="A1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -28520,13 +28521,13 @@
       <c r="A1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">

</xml_diff>

<commit_message>
statistical test for end members
</commit_message>
<xml_diff>
--- a/Data/Drifter deployment checklist.xlsx
+++ b/Data/Drifter deployment checklist.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="156">
   <si>
     <t>Swell</t>
   </si>
@@ -2157,10 +2157,10 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="L9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,6 +2273,9 @@
       <c r="A3" t="s">
         <v>126</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
       <c r="C3" s="97">
         <v>1</v>
       </c>
@@ -2333,6 +2336,9 @@
       <c r="A4" t="s">
         <v>126</v>
       </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="98">
         <f>C3+1</f>
         <v>2</v>
@@ -2394,6 +2400,9 @@
       <c r="A5" t="s">
         <v>126</v>
       </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" s="98">
         <f>C4+1</f>
         <v>3</v>
@@ -2455,6 +2464,9 @@
       <c r="A6" t="s">
         <v>117</v>
       </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
       <c r="C6" s="98">
         <f t="shared" ref="C6:C32" si="1">C5+1</f>
         <v>4</v>
@@ -2514,6 +2526,9 @@
       <c r="A7" t="s">
         <v>117</v>
       </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
       <c r="C7" s="98">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2573,6 +2588,9 @@
       <c r="A8" t="s">
         <v>117</v>
       </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
       <c r="C8" s="98">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2632,6 +2650,9 @@
       <c r="A9" t="s">
         <v>117</v>
       </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
       <c r="C9" s="98">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2695,6 +2716,9 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
       </c>
       <c r="C10" s="98">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
changed grid cell to geomorphic zones
additional analysis for revision
</commit_message>
<xml_diff>
--- a/Data/Drifter deployment checklist.xlsx
+++ b/Data/Drifter deployment checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Faga-alu-Bay-water-circulation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atm19\Documents\GitHub\Faga-alu-Bay-water-circulation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,10 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
-    <sheet name="EndmemberDefn" sheetId="6" r:id="rId2"/>
-    <sheet name="Matrix" sheetId="1" r:id="rId3"/>
-    <sheet name="NDBC NSTP6 timeseries data" sheetId="5" r:id="rId4"/>
-    <sheet name="NDBC NSTP6 data UTC no water le" sheetId="3" r:id="rId5"/>
+    <sheet name="Table (2)" sheetId="7" r:id="rId2"/>
+    <sheet name="EndmemberDefn" sheetId="6" r:id="rId3"/>
+    <sheet name="Matrix" sheetId="1" r:id="rId4"/>
+    <sheet name="NDBC NSTP6 timeseries data" sheetId="5" r:id="rId5"/>
+    <sheet name="NDBC NSTP6 data UTC no water le" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="172">
   <si>
     <t>Swell</t>
   </si>
@@ -1429,16 +1430,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2271,10 +2282,10 @@
   <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23:I32"/>
+      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4694,6 +4705,2482 @@
         <v>10</v>
       </c>
     </row>
+    <row r="35" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+    </row>
+    <row r="36" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+    </row>
+    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+    </row>
+    <row r="38" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+    </row>
+    <row r="39" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+    </row>
+    <row r="40" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+    </row>
+    <row r="41" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+    </row>
+    <row r="42" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="Q3:Q16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1"/>
+    <hyperlink ref="O1:P1" r:id="rId2" display="NSTP6"/>
+    <hyperlink ref="Q1" r:id="rId3" display="NSTP6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="M33" sqref="M33:N42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
+    <col min="18" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="8" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" customWidth="1"/>
+    <col min="22" max="22" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="31"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="102" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="121" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="121" t="s">
+        <v>159</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="121" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U2" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="97">
+        <v>1</v>
+      </c>
+      <c r="D3" s="103">
+        <v>19</v>
+      </c>
+      <c r="E3" s="84">
+        <v>41658</v>
+      </c>
+      <c r="F3" s="73">
+        <v>1300</v>
+      </c>
+      <c r="G3" s="73">
+        <v>1500</v>
+      </c>
+      <c r="H3" s="113">
+        <f>'NDBC NSTP6 timeseries data'!I4</f>
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="I3" s="28">
+        <f>H3 *0.3048</f>
+        <v>0.46908719999999998</v>
+      </c>
+      <c r="J3" s="117">
+        <f>'NDBC NSTP6 timeseries data'!I24</f>
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="K3" s="28">
+        <f>J3*0.3048</f>
+        <v>0.29687520000000001</v>
+      </c>
+      <c r="L3" s="47">
+        <f>J3-H3</f>
+        <v>-0.56499999999999995</v>
+      </c>
+      <c r="M3" s="70">
+        <f>K3 - I3</f>
+        <v>-0.17221199999999998</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="48">
+        <f>'NDBC NSTP6 timeseries data'!K25</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="P3" s="49">
+        <f>'NDBC NSTP6 timeseries data'!L25</f>
+        <v>232.5</v>
+      </c>
+      <c r="Q3" s="48">
+        <f>'NDBC NSTP6 timeseries data'!M25</f>
+        <v>3.6</v>
+      </c>
+      <c r="R3" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="112" t="s">
+        <v>154</v>
+      </c>
+      <c r="T3" s="13"/>
+      <c r="U3" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="98">
+        <f>C3+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="103">
+        <v>20</v>
+      </c>
+      <c r="E4" s="85">
+        <v>41659</v>
+      </c>
+      <c r="F4" s="72">
+        <v>1615</v>
+      </c>
+      <c r="G4" s="72">
+        <v>1730</v>
+      </c>
+      <c r="H4" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I27</f>
+        <v>1.03</v>
+      </c>
+      <c r="I4" s="28">
+        <f t="shared" ref="I4:I32" si="0">H4 *0.3048</f>
+        <v>0.313944</v>
+      </c>
+      <c r="J4" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I42</f>
+        <v>1.23</v>
+      </c>
+      <c r="K4" s="28">
+        <f t="shared" ref="K4:K32" si="1">J4*0.3048</f>
+        <v>0.37490400000000002</v>
+      </c>
+      <c r="L4" s="32">
+        <f>J4-H4</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="M4" s="70">
+        <f>K4 - I4</f>
+        <v>6.0960000000000014E-2</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K43</f>
+        <v>2.375</v>
+      </c>
+      <c r="P4" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L43</f>
+        <v>193.6875</v>
+      </c>
+      <c r="Q4" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M43</f>
+        <v>7</v>
+      </c>
+      <c r="R4" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="T4" s="109"/>
+      <c r="U4" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="98">
+        <f>C4+1</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="103">
+        <v>20</v>
+      </c>
+      <c r="E5" s="85">
+        <v>41659</v>
+      </c>
+      <c r="F5" s="72">
+        <v>1750</v>
+      </c>
+      <c r="G5" s="72">
+        <v>1900</v>
+      </c>
+      <c r="H5" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I45</f>
+        <v>1.23</v>
+      </c>
+      <c r="I5" s="28">
+        <f t="shared" si="0"/>
+        <v>0.37490400000000002</v>
+      </c>
+      <c r="J5" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I60</f>
+        <v>1.94</v>
+      </c>
+      <c r="K5" s="28">
+        <f t="shared" si="1"/>
+        <v>0.59131200000000006</v>
+      </c>
+      <c r="L5" s="32">
+        <f t="shared" ref="L5" si="2">J5-H5</f>
+        <v>0.71</v>
+      </c>
+      <c r="M5" s="70">
+        <f t="shared" ref="M5:M32" si="3">K5 - I5</f>
+        <v>0.21640800000000004</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K61</f>
+        <v>3.25</v>
+      </c>
+      <c r="P5" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L61</f>
+        <v>258.375</v>
+      </c>
+      <c r="Q5" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M61</f>
+        <v>10</v>
+      </c>
+      <c r="R5" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="T5" s="109"/>
+      <c r="U5" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="98">
+        <f t="shared" ref="C6:C32" si="4">C5+1</f>
+        <v>4</v>
+      </c>
+      <c r="D6" s="103">
+        <v>32</v>
+      </c>
+      <c r="E6" s="85">
+        <v>41671</v>
+      </c>
+      <c r="F6" s="72">
+        <v>900</v>
+      </c>
+      <c r="G6" s="72">
+        <v>1100</v>
+      </c>
+      <c r="H6" s="114">
+        <v>3.7429999999999999</v>
+      </c>
+      <c r="I6" s="28">
+        <f t="shared" si="0"/>
+        <v>1.1408663999999999</v>
+      </c>
+      <c r="J6" s="118">
+        <v>2.58</v>
+      </c>
+      <c r="K6" s="28">
+        <f t="shared" si="1"/>
+        <v>0.78638400000000008</v>
+      </c>
+      <c r="L6" s="70">
+        <f>J6-H6</f>
+        <v>-1.1629999999999998</v>
+      </c>
+      <c r="M6" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.35448239999999986</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K84</f>
+        <v>5.2725</v>
+      </c>
+      <c r="P6" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L84</f>
+        <v>96.1875</v>
+      </c>
+      <c r="Q6" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M84</f>
+        <v>11.08</v>
+      </c>
+      <c r="R6" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="T6" s="109"/>
+      <c r="U6" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="98">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="103">
+        <v>32</v>
+      </c>
+      <c r="E7" s="85">
+        <v>41671</v>
+      </c>
+      <c r="F7" s="72">
+        <v>1130</v>
+      </c>
+      <c r="G7" s="72">
+        <v>1300</v>
+      </c>
+      <c r="H7" s="114">
+        <v>2.2280000000000002</v>
+      </c>
+      <c r="I7" s="28">
+        <f t="shared" si="0"/>
+        <v>0.6790944000000001</v>
+      </c>
+      <c r="J7" s="118">
+        <v>0.879</v>
+      </c>
+      <c r="K7" s="28">
+        <f t="shared" si="1"/>
+        <v>0.26791920000000002</v>
+      </c>
+      <c r="L7" s="70">
+        <f>J7-H7</f>
+        <v>-1.3490000000000002</v>
+      </c>
+      <c r="M7" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.41117520000000007</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K102</f>
+        <v>5.6875</v>
+      </c>
+      <c r="P7" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L102</f>
+        <v>100.25</v>
+      </c>
+      <c r="Q7" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M102</f>
+        <v>13</v>
+      </c>
+      <c r="R7" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="T7" s="109"/>
+      <c r="U7" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="98">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="103">
+        <v>32</v>
+      </c>
+      <c r="E8" s="85">
+        <v>41671</v>
+      </c>
+      <c r="F8" s="72">
+        <v>1700</v>
+      </c>
+      <c r="G8" s="72">
+        <v>1900</v>
+      </c>
+      <c r="H8" s="114">
+        <v>1.512</v>
+      </c>
+      <c r="I8" s="28">
+        <f t="shared" si="0"/>
+        <v>0.46085760000000003</v>
+      </c>
+      <c r="J8" s="118">
+        <v>3.222</v>
+      </c>
+      <c r="K8" s="28">
+        <f t="shared" si="1"/>
+        <v>0.98206560000000009</v>
+      </c>
+      <c r="L8" s="32">
+        <f t="shared" ref="L8:L32" si="5">J8-H8</f>
+        <v>1.71</v>
+      </c>
+      <c r="M8" s="70">
+        <f t="shared" si="3"/>
+        <v>0.52120800000000012</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K125</f>
+        <v>4.2380952380952381</v>
+      </c>
+      <c r="P8" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L125</f>
+        <v>187.95238095238096</v>
+      </c>
+      <c r="Q8" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M125</f>
+        <v>13</v>
+      </c>
+      <c r="R8" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="T8" s="109"/>
+      <c r="U8" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="98">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="103">
+        <v>39</v>
+      </c>
+      <c r="E9" s="85">
+        <v>41678</v>
+      </c>
+      <c r="F9" s="72">
+        <v>1415</v>
+      </c>
+      <c r="G9" s="72">
+        <v>1545</v>
+      </c>
+      <c r="H9" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I127</f>
+        <v>3.1</v>
+      </c>
+      <c r="I9" s="28">
+        <f t="shared" si="0"/>
+        <v>0.94488000000000005</v>
+      </c>
+      <c r="J9" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I143</f>
+        <v>3.45</v>
+      </c>
+      <c r="K9" s="28">
+        <f t="shared" si="1"/>
+        <v>1.0515600000000001</v>
+      </c>
+      <c r="L9" s="32">
+        <f t="shared" si="5"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="M9" s="70">
+        <f t="shared" si="3"/>
+        <v>0.10668</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K144</f>
+        <v>5.2352941176470589</v>
+      </c>
+      <c r="P9" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L144</f>
+        <v>140.41176470588235</v>
+      </c>
+      <c r="Q9" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M144</f>
+        <v>18</v>
+      </c>
+      <c r="R9" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T9" s="109"/>
+      <c r="U9" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" s="88" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="98">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="103">
+        <v>39</v>
+      </c>
+      <c r="E10" s="85">
+        <v>41678</v>
+      </c>
+      <c r="F10" s="72">
+        <v>1605</v>
+      </c>
+      <c r="G10" s="72">
+        <v>1800</v>
+      </c>
+      <c r="H10" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I146</f>
+        <v>3.33</v>
+      </c>
+      <c r="I10" s="28">
+        <f t="shared" si="0"/>
+        <v>1.0149840000000001</v>
+      </c>
+      <c r="J10" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I167</f>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="K10" s="28">
+        <f t="shared" si="1"/>
+        <v>0.77114399999999994</v>
+      </c>
+      <c r="L10" s="70">
+        <f t="shared" si="5"/>
+        <v>-0.80000000000000027</v>
+      </c>
+      <c r="M10" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.24384000000000017</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K168</f>
+        <v>6.0454545454545459</v>
+      </c>
+      <c r="P10" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L168</f>
+        <v>144.13636363636363</v>
+      </c>
+      <c r="Q10" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M168</f>
+        <v>20</v>
+      </c>
+      <c r="R10" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T10" s="109"/>
+      <c r="U10" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W10" s="88" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="98">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="103">
+        <v>47</v>
+      </c>
+      <c r="E11" s="85">
+        <v>41686</v>
+      </c>
+      <c r="F11" s="72">
+        <v>1654</v>
+      </c>
+      <c r="G11" s="72">
+        <v>1846</v>
+      </c>
+      <c r="H11" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I170</f>
+        <v>2.39</v>
+      </c>
+      <c r="I11" s="28">
+        <f t="shared" si="0"/>
+        <v>0.72847200000000012</v>
+      </c>
+      <c r="J11" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I189</f>
+        <v>3.25</v>
+      </c>
+      <c r="K11" s="28">
+        <f t="shared" si="1"/>
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="L11" s="32">
+        <f t="shared" si="5"/>
+        <v>0.85999999999999988</v>
+      </c>
+      <c r="M11" s="70">
+        <f t="shared" si="3"/>
+        <v>0.26212799999999992</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K190</f>
+        <v>3.25</v>
+      </c>
+      <c r="P11" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L190</f>
+        <v>168.8</v>
+      </c>
+      <c r="Q11" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M190</f>
+        <v>9</v>
+      </c>
+      <c r="R11" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="S11" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T11" s="109"/>
+      <c r="U11" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W11" s="88" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="98">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="103">
+        <v>48</v>
+      </c>
+      <c r="E12" s="85">
+        <v>41687</v>
+      </c>
+      <c r="F12" s="72">
+        <v>1245</v>
+      </c>
+      <c r="G12" s="72">
+        <v>1500</v>
+      </c>
+      <c r="H12" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I192</f>
+        <v>1.62</v>
+      </c>
+      <c r="I12" s="28">
+        <f t="shared" si="0"/>
+        <v>0.49377600000000005</v>
+      </c>
+      <c r="J12" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I215</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K12" s="28">
+        <f t="shared" si="1"/>
+        <v>0.33832800000000007</v>
+      </c>
+      <c r="L12" s="70">
+        <f t="shared" si="5"/>
+        <v>-0.51</v>
+      </c>
+      <c r="M12" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.15544799999999998</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K216</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="P12" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L216</f>
+        <v>79.958333333333329</v>
+      </c>
+      <c r="Q12" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M216</f>
+        <v>28</v>
+      </c>
+      <c r="R12" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T12" s="109"/>
+      <c r="U12" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="88" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="98">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="103">
+        <v>48</v>
+      </c>
+      <c r="E13" s="85">
+        <v>41687</v>
+      </c>
+      <c r="F13" s="72">
+        <v>1530</v>
+      </c>
+      <c r="G13" s="72">
+        <v>1700</v>
+      </c>
+      <c r="H13" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I218</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I13" s="28">
+        <f t="shared" si="0"/>
+        <v>0.347472</v>
+      </c>
+      <c r="J13" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I236</f>
+        <v>1.59</v>
+      </c>
+      <c r="K13" s="28">
+        <f t="shared" si="1"/>
+        <v>0.48463200000000006</v>
+      </c>
+      <c r="L13" s="32">
+        <f t="shared" si="5"/>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="M13" s="70">
+        <f t="shared" si="3"/>
+        <v>0.13716000000000006</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K237</f>
+        <v>5.8947368421052628</v>
+      </c>
+      <c r="P13" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L237</f>
+        <v>101.36842105263158</v>
+      </c>
+      <c r="Q13" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M237</f>
+        <v>20</v>
+      </c>
+      <c r="R13" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S13" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T13" s="109"/>
+      <c r="U13" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W13" s="88" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="98">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="D14" s="103">
+        <v>48</v>
+      </c>
+      <c r="E14" s="85">
+        <v>41687</v>
+      </c>
+      <c r="F14" s="72">
+        <v>1710</v>
+      </c>
+      <c r="G14" s="72">
+        <v>1840</v>
+      </c>
+      <c r="H14" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I239</f>
+        <v>1.62</v>
+      </c>
+      <c r="I14" s="28">
+        <f t="shared" si="0"/>
+        <v>0.49377600000000005</v>
+      </c>
+      <c r="J14" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I256</f>
+        <v>2.56</v>
+      </c>
+      <c r="K14" s="28">
+        <f t="shared" si="1"/>
+        <v>0.78028800000000009</v>
+      </c>
+      <c r="L14" s="32">
+        <f t="shared" si="5"/>
+        <v>0.94</v>
+      </c>
+      <c r="M14" s="70">
+        <f t="shared" si="3"/>
+        <v>0.28651200000000004</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K257</f>
+        <v>5.166666666666667</v>
+      </c>
+      <c r="P14" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L257</f>
+        <v>89.888888888888886</v>
+      </c>
+      <c r="Q14" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M257</f>
+        <v>15</v>
+      </c>
+      <c r="R14" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S14" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T14" s="109"/>
+      <c r="U14" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W14" s="88" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="98">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="D15" s="103">
+        <v>49</v>
+      </c>
+      <c r="E15" s="85">
+        <v>41688</v>
+      </c>
+      <c r="F15" s="72">
+        <v>1245</v>
+      </c>
+      <c r="G15" s="72">
+        <v>1445</v>
+      </c>
+      <c r="H15" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I259</f>
+        <v>2.09</v>
+      </c>
+      <c r="I15" s="28">
+        <f t="shared" si="0"/>
+        <v>0.63703200000000004</v>
+      </c>
+      <c r="J15" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I280</f>
+        <v>1.26</v>
+      </c>
+      <c r="K15" s="28">
+        <f t="shared" si="1"/>
+        <v>0.384048</v>
+      </c>
+      <c r="L15" s="70">
+        <f t="shared" si="5"/>
+        <v>-0.82999999999999985</v>
+      </c>
+      <c r="M15" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.25298400000000004</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O15" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K281</f>
+        <v>4.9090909090909092</v>
+      </c>
+      <c r="P15" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L281</f>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="Q15" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M281</f>
+        <v>14</v>
+      </c>
+      <c r="R15" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T15" s="109"/>
+      <c r="U15" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" s="88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="99">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="D16" s="103">
+        <v>49</v>
+      </c>
+      <c r="E16" s="86">
+        <v>41688</v>
+      </c>
+      <c r="F16" s="76">
+        <v>1445</v>
+      </c>
+      <c r="G16" s="76">
+        <v>1700</v>
+      </c>
+      <c r="H16" s="115">
+        <f>'NDBC NSTP6 timeseries data'!I283</f>
+        <v>1.3</v>
+      </c>
+      <c r="I16" s="28">
+        <f t="shared" si="0"/>
+        <v>0.39624000000000004</v>
+      </c>
+      <c r="J16" s="119">
+        <f>'NDBC NSTP6 timeseries data'!I306</f>
+        <v>1.37</v>
+      </c>
+      <c r="K16" s="28">
+        <f t="shared" si="1"/>
+        <v>0.41757600000000006</v>
+      </c>
+      <c r="L16" s="78">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000062E-2</v>
+      </c>
+      <c r="M16" s="70">
+        <f t="shared" si="3"/>
+        <v>2.1336000000000022E-2</v>
+      </c>
+      <c r="N16" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" s="79">
+        <f>'NDBC NSTP6 timeseries data'!K307</f>
+        <v>4.708333333333333</v>
+      </c>
+      <c r="P16" s="80">
+        <f>'NDBC NSTP6 timeseries data'!L307</f>
+        <v>194.41666666666666</v>
+      </c>
+      <c r="Q16" s="79">
+        <f>'NDBC NSTP6 timeseries data'!M307</f>
+        <v>15</v>
+      </c>
+      <c r="R16" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T16" s="110"/>
+      <c r="U16" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" s="88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="98">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="D17" s="103">
+        <v>50</v>
+      </c>
+      <c r="E17" s="85">
+        <v>41689</v>
+      </c>
+      <c r="F17" s="72">
+        <v>1205</v>
+      </c>
+      <c r="G17" s="72">
+        <v>1440</v>
+      </c>
+      <c r="H17" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I309</f>
+        <v>2.8809999999999998</v>
+      </c>
+      <c r="I17" s="28">
+        <f t="shared" si="0"/>
+        <v>0.87812879999999993</v>
+      </c>
+      <c r="J17" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I336</f>
+        <v>1.516</v>
+      </c>
+      <c r="K17" s="28">
+        <f t="shared" si="1"/>
+        <v>0.46207680000000001</v>
+      </c>
+      <c r="L17" s="90">
+        <f t="shared" si="5"/>
+        <v>-1.3649999999999998</v>
+      </c>
+      <c r="M17" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.41605199999999992</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K337</f>
+        <v>5.7757142857142858</v>
+      </c>
+      <c r="P17" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L337</f>
+        <v>39.857142857142854</v>
+      </c>
+      <c r="Q17" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M337</f>
+        <v>11.47</v>
+      </c>
+      <c r="R17" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T17" s="109"/>
+      <c r="U17" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V17" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="98">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="D18" s="103">
+        <v>50</v>
+      </c>
+      <c r="E18" s="85">
+        <v>41689</v>
+      </c>
+      <c r="F18" s="72">
+        <v>1445</v>
+      </c>
+      <c r="G18" s="72">
+        <v>1720</v>
+      </c>
+      <c r="H18" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I339</f>
+        <v>1.516</v>
+      </c>
+      <c r="I18" s="28">
+        <f t="shared" si="0"/>
+        <v>0.46207680000000001</v>
+      </c>
+      <c r="J18" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I365</f>
+        <v>1.24</v>
+      </c>
+      <c r="K18" s="28">
+        <f t="shared" si="1"/>
+        <v>0.37795200000000001</v>
+      </c>
+      <c r="L18" s="90">
+        <f t="shared" si="5"/>
+        <v>-0.27600000000000002</v>
+      </c>
+      <c r="M18" s="70">
+        <f t="shared" si="3"/>
+        <v>-8.41248E-2</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K366</f>
+        <v>6.565555555555556</v>
+      </c>
+      <c r="P18" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L366</f>
+        <v>54.407407407407405</v>
+      </c>
+      <c r="Q18" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M366</f>
+        <v>14.77</v>
+      </c>
+      <c r="R18" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T18" s="109"/>
+      <c r="U18" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V18" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="98">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="D19" s="103">
+        <v>51</v>
+      </c>
+      <c r="E19" s="85">
+        <v>41690</v>
+      </c>
+      <c r="F19" s="72">
+        <v>840</v>
+      </c>
+      <c r="G19" s="72">
+        <v>1045</v>
+      </c>
+      <c r="H19" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I368</f>
+        <v>2.52</v>
+      </c>
+      <c r="I19" s="28">
+        <f t="shared" si="0"/>
+        <v>0.768096</v>
+      </c>
+      <c r="J19" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I389</f>
+        <v>3.15</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" si="1"/>
+        <v>0.96011999999999997</v>
+      </c>
+      <c r="L19" s="78">
+        <f t="shared" si="5"/>
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="M19" s="70">
+        <f t="shared" si="3"/>
+        <v>0.19202399999999997</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K390</f>
+        <v>4.8181818181818183</v>
+      </c>
+      <c r="P19" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L390</f>
+        <v>290.22727272727275</v>
+      </c>
+      <c r="Q19" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M390</f>
+        <v>13</v>
+      </c>
+      <c r="R19" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T19" s="109"/>
+      <c r="U19" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="98">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="D20" s="103">
+        <v>51</v>
+      </c>
+      <c r="E20" s="85">
+        <v>41690</v>
+      </c>
+      <c r="F20" s="72">
+        <v>1100</v>
+      </c>
+      <c r="G20" s="72">
+        <v>1200</v>
+      </c>
+      <c r="H20" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I392</f>
+        <v>3.2</v>
+      </c>
+      <c r="I20" s="28">
+        <f t="shared" si="0"/>
+        <v>0.97536000000000012</v>
+      </c>
+      <c r="J20" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I402</f>
+        <v>3.05</v>
+      </c>
+      <c r="K20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.92964000000000002</v>
+      </c>
+      <c r="L20" s="90">
+        <f t="shared" si="5"/>
+        <v>-0.15000000000000036</v>
+      </c>
+      <c r="M20" s="70">
+        <f t="shared" si="3"/>
+        <v>-4.5720000000000094E-2</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K403</f>
+        <v>4.2727272727272725</v>
+      </c>
+      <c r="P20" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L403</f>
+        <v>117.18181818181819</v>
+      </c>
+      <c r="Q20" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M403</f>
+        <v>11</v>
+      </c>
+      <c r="R20" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T20" s="109"/>
+      <c r="U20" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V20" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="98">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="D21" s="103">
+        <v>51</v>
+      </c>
+      <c r="E21" s="85">
+        <v>41690</v>
+      </c>
+      <c r="F21" s="72">
+        <v>1210</v>
+      </c>
+      <c r="G21" s="72">
+        <v>1430</v>
+      </c>
+      <c r="H21" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I405</f>
+        <v>3.02</v>
+      </c>
+      <c r="I21" s="28">
+        <f t="shared" si="0"/>
+        <v>0.92049600000000009</v>
+      </c>
+      <c r="J21" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I429</f>
+        <v>2.06</v>
+      </c>
+      <c r="K21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.627888</v>
+      </c>
+      <c r="L21" s="90">
+        <f t="shared" si="5"/>
+        <v>-0.96</v>
+      </c>
+      <c r="M21" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.29260800000000009</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K430</f>
+        <v>2.96</v>
+      </c>
+      <c r="P21" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L430</f>
+        <v>237.8</v>
+      </c>
+      <c r="Q21" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M430</f>
+        <v>12</v>
+      </c>
+      <c r="R21" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T21" s="109"/>
+      <c r="U21" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V21" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="98">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="103">
+        <v>51</v>
+      </c>
+      <c r="E22" s="85">
+        <v>41690</v>
+      </c>
+      <c r="F22" s="72">
+        <v>1500</v>
+      </c>
+      <c r="G22" s="72">
+        <v>1630</v>
+      </c>
+      <c r="H22" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I432</f>
+        <v>1.85</v>
+      </c>
+      <c r="I22" s="28">
+        <f t="shared" si="0"/>
+        <v>0.56388000000000005</v>
+      </c>
+      <c r="J22" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I447</f>
+        <v>1.29</v>
+      </c>
+      <c r="K22" s="28">
+        <f t="shared" si="1"/>
+        <v>0.39319200000000004</v>
+      </c>
+      <c r="L22" s="90">
+        <f t="shared" si="5"/>
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="M22" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.17068800000000001</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K448</f>
+        <v>5.9375</v>
+      </c>
+      <c r="P22" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L448</f>
+        <v>290</v>
+      </c>
+      <c r="Q22" s="28">
+        <f>'NDBC NSTP6 timeseries data'!M448</f>
+        <v>13</v>
+      </c>
+      <c r="R22" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="S22" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T22" s="109"/>
+      <c r="U22" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="98">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="D23" s="103">
+        <v>52</v>
+      </c>
+      <c r="E23" s="85">
+        <v>41691</v>
+      </c>
+      <c r="F23" s="11">
+        <v>920</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1040</v>
+      </c>
+      <c r="H23" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I450</f>
+        <v>2.37</v>
+      </c>
+      <c r="I23" s="28">
+        <f t="shared" si="0"/>
+        <v>0.72237600000000002</v>
+      </c>
+      <c r="J23" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I464</f>
+        <v>2.97</v>
+      </c>
+      <c r="K23" s="28">
+        <f t="shared" si="1"/>
+        <v>0.90525600000000006</v>
+      </c>
+      <c r="L23" s="78">
+        <f t="shared" si="5"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="M23" s="70">
+        <f t="shared" si="3"/>
+        <v>0.18288000000000004</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K465</f>
+        <v>2.8666666666666667</v>
+      </c>
+      <c r="P23" s="11">
+        <f>'NDBC NSTP6 timeseries data'!L465</f>
+        <v>253</v>
+      </c>
+      <c r="Q23" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M465</f>
+        <v>11</v>
+      </c>
+      <c r="R23" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T23" s="111"/>
+      <c r="U23" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="98">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="D24" s="103">
+        <v>52</v>
+      </c>
+      <c r="E24" s="85">
+        <v>41691</v>
+      </c>
+      <c r="F24" s="11">
+        <v>1040</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1145</v>
+      </c>
+      <c r="H24" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I467</f>
+        <v>3.01</v>
+      </c>
+      <c r="I24" s="28">
+        <f t="shared" si="0"/>
+        <v>0.91744799999999993</v>
+      </c>
+      <c r="J24" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I479</f>
+        <v>3.29</v>
+      </c>
+      <c r="K24" s="28">
+        <f t="shared" si="1"/>
+        <v>1.0027920000000001</v>
+      </c>
+      <c r="L24" s="78">
+        <f t="shared" si="5"/>
+        <v>0.28000000000000025</v>
+      </c>
+      <c r="M24" s="70">
+        <f t="shared" si="3"/>
+        <v>8.5344000000000197E-2</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K480</f>
+        <v>3.8461538461538463</v>
+      </c>
+      <c r="P24" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L480</f>
+        <v>111.15384615384616</v>
+      </c>
+      <c r="Q24" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M480</f>
+        <v>11</v>
+      </c>
+      <c r="R24" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S24" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T24" s="12"/>
+      <c r="U24" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="99">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="103">
+        <v>52</v>
+      </c>
+      <c r="E25" s="86">
+        <v>41691</v>
+      </c>
+      <c r="F25" s="77">
+        <v>1300</v>
+      </c>
+      <c r="G25" s="77">
+        <v>1400</v>
+      </c>
+      <c r="H25" s="115">
+        <f>'NDBC NSTP6 timeseries data'!I482</f>
+        <v>3.24</v>
+      </c>
+      <c r="I25" s="28">
+        <f t="shared" si="0"/>
+        <v>0.9875520000000001</v>
+      </c>
+      <c r="J25" s="119">
+        <f>'NDBC NSTP6 timeseries data'!I492</f>
+        <v>2.97</v>
+      </c>
+      <c r="K25" s="28">
+        <f t="shared" si="1"/>
+        <v>0.90525600000000006</v>
+      </c>
+      <c r="L25" s="90">
+        <f t="shared" si="5"/>
+        <v>-0.27</v>
+      </c>
+      <c r="M25" s="70">
+        <f t="shared" si="3"/>
+        <v>-8.2296000000000036E-2</v>
+      </c>
+      <c r="N25" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="O25" s="79">
+        <f>'NDBC NSTP6 timeseries data'!K493</f>
+        <v>3</v>
+      </c>
+      <c r="P25" s="80">
+        <f>'NDBC NSTP6 timeseries data'!L493</f>
+        <v>193.45454545454547</v>
+      </c>
+      <c r="Q25" s="77">
+        <f>'NDBC NSTP6 timeseries data'!M493</f>
+        <v>16</v>
+      </c>
+      <c r="R25" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T25" s="81"/>
+      <c r="U25" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="V25" s="89" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="98">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="D26" s="103">
+        <v>52</v>
+      </c>
+      <c r="E26" s="85">
+        <v>41691</v>
+      </c>
+      <c r="F26" s="11">
+        <v>1500</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1550</v>
+      </c>
+      <c r="H26" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I495</f>
+        <v>2.39</v>
+      </c>
+      <c r="I26" s="28">
+        <f t="shared" si="0"/>
+        <v>0.72847200000000012</v>
+      </c>
+      <c r="J26" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I505</f>
+        <v>1.86</v>
+      </c>
+      <c r="K26" s="28">
+        <f t="shared" si="1"/>
+        <v>0.5669280000000001</v>
+      </c>
+      <c r="L26" s="70">
+        <f t="shared" si="5"/>
+        <v>-0.53</v>
+      </c>
+      <c r="M26" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.16154400000000002</v>
+      </c>
+      <c r="N26" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O26" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K506</f>
+        <v>3.7272727272727271</v>
+      </c>
+      <c r="P26" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L506</f>
+        <v>152.27272727272728</v>
+      </c>
+      <c r="Q26" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M506</f>
+        <v>11</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V26" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="98">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="D27" s="103">
+        <v>53</v>
+      </c>
+      <c r="E27" s="85">
+        <v>41692</v>
+      </c>
+      <c r="F27" s="11">
+        <v>1100</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1215</v>
+      </c>
+      <c r="H27" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I508</f>
+        <v>2.71</v>
+      </c>
+      <c r="I27" s="28">
+        <f t="shared" si="0"/>
+        <v>0.82600800000000008</v>
+      </c>
+      <c r="J27" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I521</f>
+        <v>3.17</v>
+      </c>
+      <c r="K27" s="28">
+        <f t="shared" si="1"/>
+        <v>0.96621600000000007</v>
+      </c>
+      <c r="L27" s="32">
+        <f t="shared" si="5"/>
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="M27" s="70">
+        <f t="shared" si="3"/>
+        <v>0.140208</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27" s="11">
+        <f>'NDBC NSTP6 timeseries data'!K522</f>
+        <v>5.5</v>
+      </c>
+      <c r="P27" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L522</f>
+        <v>313.85714285714283</v>
+      </c>
+      <c r="Q27" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M522</f>
+        <v>14</v>
+      </c>
+      <c r="R27" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S27" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T27" s="11"/>
+      <c r="U27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V27" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="98">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="D28" s="103">
+        <v>53</v>
+      </c>
+      <c r="E28" s="85">
+        <v>41692</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1220</v>
+      </c>
+      <c r="G28" s="11">
+        <v>1315</v>
+      </c>
+      <c r="H28" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I524</f>
+        <v>3.19</v>
+      </c>
+      <c r="I28" s="28">
+        <f t="shared" si="0"/>
+        <v>0.97231200000000007</v>
+      </c>
+      <c r="J28" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I535</f>
+        <v>3.37</v>
+      </c>
+      <c r="K28" s="28">
+        <f t="shared" si="1"/>
+        <v>1.0271760000000001</v>
+      </c>
+      <c r="L28" s="32">
+        <f t="shared" si="5"/>
+        <v>0.18000000000000016</v>
+      </c>
+      <c r="M28" s="70">
+        <f t="shared" si="3"/>
+        <v>5.4864000000000024E-2</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K536</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="P28" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L536</f>
+        <v>301.5</v>
+      </c>
+      <c r="Q28" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M536</f>
+        <v>12</v>
+      </c>
+      <c r="R28" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S28" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T28" s="11"/>
+      <c r="U28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V28" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="98">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="D29" s="103">
+        <v>53</v>
+      </c>
+      <c r="E29" s="85">
+        <v>41692</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1600</v>
+      </c>
+      <c r="G29" s="11">
+        <v>1700</v>
+      </c>
+      <c r="H29" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I538</f>
+        <v>2.44</v>
+      </c>
+      <c r="I29" s="28">
+        <f t="shared" si="0"/>
+        <v>0.74371200000000004</v>
+      </c>
+      <c r="J29" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I548</f>
+        <v>1.92</v>
+      </c>
+      <c r="K29" s="28">
+        <f t="shared" si="1"/>
+        <v>0.58521599999999996</v>
+      </c>
+      <c r="L29" s="70">
+        <f t="shared" si="5"/>
+        <v>-0.52</v>
+      </c>
+      <c r="M29" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.15849600000000008</v>
+      </c>
+      <c r="N29" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O29" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K549</f>
+        <v>4.1818181818181817</v>
+      </c>
+      <c r="P29" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L549</f>
+        <v>310.90909090909093</v>
+      </c>
+      <c r="Q29" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M549</f>
+        <v>10</v>
+      </c>
+      <c r="R29" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S29" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T29" s="11"/>
+      <c r="U29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V29" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="98">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="D30" s="103">
+        <v>53</v>
+      </c>
+      <c r="E30" s="85">
+        <v>41692</v>
+      </c>
+      <c r="F30" s="11">
+        <v>1700</v>
+      </c>
+      <c r="G30" s="11">
+        <v>1845</v>
+      </c>
+      <c r="H30" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I551</f>
+        <v>1.92</v>
+      </c>
+      <c r="I30" s="28">
+        <f t="shared" si="0"/>
+        <v>0.58521599999999996</v>
+      </c>
+      <c r="J30" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I569</f>
+        <v>1.21</v>
+      </c>
+      <c r="K30" s="28">
+        <f t="shared" si="1"/>
+        <v>0.36880800000000002</v>
+      </c>
+      <c r="L30" s="70">
+        <f t="shared" si="5"/>
+        <v>-0.71</v>
+      </c>
+      <c r="M30" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.21640799999999993</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K570</f>
+        <v>2</v>
+      </c>
+      <c r="P30" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L570</f>
+        <v>242.47368421052633</v>
+      </c>
+      <c r="Q30" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M570</f>
+        <v>10</v>
+      </c>
+      <c r="R30" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S30" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="T30" s="11"/>
+      <c r="U30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V30" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="98">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="D31" s="103">
+        <v>54</v>
+      </c>
+      <c r="E31" s="85">
+        <v>41693</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1040</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1210</v>
+      </c>
+      <c r="H31" s="114">
+        <f>'NDBC NSTP6 timeseries data'!I572</f>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="I31" s="28">
+        <f t="shared" si="0"/>
+        <v>0.61264799999999997</v>
+      </c>
+      <c r="J31" s="118">
+        <f>'NDBC NSTP6 timeseries data'!I587</f>
+        <v>2.9</v>
+      </c>
+      <c r="K31" s="28">
+        <f t="shared" si="1"/>
+        <v>0.88392000000000004</v>
+      </c>
+      <c r="L31" s="70">
+        <f t="shared" si="5"/>
+        <v>0.89000000000000012</v>
+      </c>
+      <c r="M31" s="70">
+        <f t="shared" si="3"/>
+        <v>0.27127200000000007</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O31" s="28">
+        <f>'NDBC NSTP6 timeseries data'!K588</f>
+        <v>7.1875</v>
+      </c>
+      <c r="P31" s="27">
+        <f>'NDBC NSTP6 timeseries data'!L588</f>
+        <v>304.1875</v>
+      </c>
+      <c r="Q31" s="11">
+        <f>'NDBC NSTP6 timeseries data'!M588</f>
+        <v>15</v>
+      </c>
+      <c r="R31" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="S31" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="V31" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="100">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D32" s="104">
+        <v>54</v>
+      </c>
+      <c r="E32" s="101">
+        <v>41693</v>
+      </c>
+      <c r="F32" s="91">
+        <v>1210</v>
+      </c>
+      <c r="G32" s="91">
+        <v>1255</v>
+      </c>
+      <c r="H32" s="116">
+        <f>'NDBC NSTP6 timeseries data'!I590</f>
+        <v>2.9</v>
+      </c>
+      <c r="I32" s="28">
+        <f t="shared" si="0"/>
+        <v>0.88392000000000004</v>
+      </c>
+      <c r="J32" s="120">
+        <f>'NDBC NSTP6 timeseries data'!I599</f>
+        <v>3.27</v>
+      </c>
+      <c r="K32" s="28">
+        <f t="shared" si="1"/>
+        <v>0.99669600000000003</v>
+      </c>
+      <c r="L32" s="92">
+        <f t="shared" si="5"/>
+        <v>0.37000000000000011</v>
+      </c>
+      <c r="M32" s="70">
+        <f t="shared" si="3"/>
+        <v>0.11277599999999999</v>
+      </c>
+      <c r="N32" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="O32" s="93">
+        <f>'NDBC NSTP6 timeseries data'!K600</f>
+        <v>5.2857142857142856</v>
+      </c>
+      <c r="P32" s="94">
+        <f>'NDBC NSTP6 timeseries data'!L600</f>
+        <v>260.28571428571428</v>
+      </c>
+      <c r="Q32" s="91">
+        <f>'NDBC NSTP6 timeseries data'!M600</f>
+        <v>11</v>
+      </c>
+      <c r="R32" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="S32" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="T32" s="16"/>
+      <c r="U32" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="V32" s="96" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="33" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
         <v>162</v>
@@ -4729,7 +7216,7 @@
       <c r="M36" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="N36" s="124">
+      <c r="N36" s="123">
         <f>COUNTIF(N11:N32,  "falling")</f>
         <v>11</v>
       </c>
@@ -4747,7 +7234,7 @@
       <c r="M38" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="N38" s="124">
+      <c r="N38" s="123">
         <f>COUNTIF(N17:N22,  "falling")</f>
         <v>5</v>
       </c>
@@ -4765,7 +7252,7 @@
       <c r="M40" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="N40" s="124">
+      <c r="N40" s="123">
         <f>COUNTIF(N11:N16,  "falling")</f>
         <v>2</v>
       </c>
@@ -4783,7 +7270,7 @@
       <c r="M42" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="N42" s="124">
+      <c r="N42" s="123">
         <f>COUNTIF(N23:N32,  "falling")</f>
         <v>4</v>
       </c>
@@ -4804,7 +7291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -4879,7 +7366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
@@ -5223,7 +7710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y600"/>
   <sheetViews>
@@ -5255,11 +7742,11 @@
       <c r="A1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
@@ -29106,7 +31593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z61"/>
   <sheetViews>
@@ -29137,13 +31624,13 @@
       <c r="A1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="123" t="s">
+      <c r="H1" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">

</xml_diff>